<commit_message>
Update ATT&CK Enterprise Techniques with MulVAL IR.xlsx
New IRs (Ext38)
</commit_message>
<xml_diff>
--- a/ATT&CK Enterprise Techniques with MulVAL IR.xlsx
+++ b/ATT&CK Enterprise Techniques with MulVAL IR.xlsx
@@ -4,24 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="585" windowWidth="27660" windowHeight="11955"/>
+    <workbookView xWindow="510" yWindow="525" windowWidth="26580" windowHeight="10935"/>
   </bookViews>
   <sheets>
     <sheet name="Enterprise ATT&amp;CK" sheetId="1" r:id="rId1"/>
-    <sheet name="Sum" sheetId="2" r:id="rId2"/>
+    <sheet name="Expressed Tactics" sheetId="2" r:id="rId2"/>
     <sheet name="Techniques in Multi-Tactics" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mhMB53q8WSyGsRGIPSoWlXgh96zJQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mj6VvYWCsLllCF+uqfa1pvh+qzw7A=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="403">
   <si>
     <t>Technique</t>
   </si>
@@ -453,8 +453,8 @@
   <si>
     <t>stealthyBridgeExists(Vm_1, Vm_2, Host, stealthyBridge_id) :-
   execCode(Vm_1, _user),
-  ResideOn(Vm_1, Host),
-  ResideOn(Vm_2, Host).</t>
+  resideOn(Vm_1, Host),
+  resideOn(Vm_2, Host).</t>
   </si>
   <si>
     <t>Defense Evasion</t>
@@ -925,6 +925,12 @@
     <t>Exploitation of Remote Services</t>
   </si>
   <si>
+    <t>stealthyBridgeExists(Vm_1, Vm_2, Host, stealthyBridge_id) :-
+  execCode(Vm_1, _user),
+  ResideOn(Vm_1, Host),
+  ResideOn(Vm_2, Host).</t>
+  </si>
+  <si>
     <t>Internal Spearphishing</t>
   </si>
   <si>
@@ -1392,6 +1398,442 @@
   manInTheMiddle(Host, _, Tgt).</t>
   </si>
   <si>
+    <t>Specific to Machine Learning, doesn't exist in MITRE yet</t>
+  </si>
+  <si>
+    <t>evasionAttack4(Principal, PiplineID, ModelID, tampering) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, evasionAttackVulnerability),
+  completeKnowledge3(Principal, PiplineID, ModelID).</t>
+  </si>
+  <si>
+    <t>Ext38</t>
+  </si>
+  <si>
+    <t>evasionAttack4(Principal, PiplineID, ModelID, tampering) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, evasionAttackVulnerability),
+  queryAccess5(Principal, PiplineID, ModelID, score, full),
+  taskKnowledge4(Principal, PiplineID, ModelID, KnowledgeLevel).</t>
+  </si>
+  <si>
+    <t>evasionAttack4(Principal, PiplineID, ModelID, tampering) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, evasionAttackVulnerability),
+  queryAccess5(Principal, PiplineID, ModelID, decision, full),
+  taskKnowledge4(Principal, PiplineID, ModelID, KnowledgeLevel).</t>
+  </si>
+  <si>
+    <t>evasionAttack4(Principal, PiplineID, ModelID, tampering) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, evasionAttackVulnerability),
+  surrogateDataAccess4(Principal, PiplineID, ModelID, limited),
+  queryAccess5(Principal, PiplineID, ModelID, decision, full),
+  dataPropertiesKnowledge4(Principal, PiplineID, ModelID, full),
+  taskKnowledge4(Principal, PiplineID, ModelID, full).</t>
+  </si>
+  <si>
+    <t>evasionAttack4(Principal, PiplineID, ModelID, tampering) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, evasionAttackVulnerability),
+  queryAccess5(Principal, PiplineID, ModelID, decision, full),
+  trainingDataKnowledge5(Principal, PiplineID, ModelID, TrainingDataID, full),
+  rawDataKnowledge5(Principal, PiplineID, ModelID, RawDataID, full),
+  dataPropertiesKnowledge4(Principal, PiplineID, ModelID, full),
+  taskKnowledge4(Principal, PiplineID, ModelID, full).</t>
+  </si>
+  <si>
+    <t>evasionAttack4(Principal, PiplineID, ModelID, tampering) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  modelRetrainedContinuously_p2(PiplineID,  ModelID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, evasionAttackVulnerability),
+  rawDataAccess6(Principal, PiplineID, ModelID, RawDataID, write, limited),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, write,limited),
+  labeledDataAccess6(Principal, PiplineID, ModelID, LabeledDataID, write, limited),
+  queryAccess5(Principal, PiplineID, ModelID, decision, limited),
+  completeKnowledge3(Principal, PiplineID, ModelID).</t>
+  </si>
+  <si>
+    <t>evasionAttack4(Principal, PiplineID, ModelID, tampering) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  modelRetrainedContinuously_p2(PiplineID, ModelID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, evasionAttackVulnerability),
+  rawDataAccess6(Principal, PiplineID, ModelID, RawDataID, _, limited),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, write, limited),
+  labeledDataAccess6(Principal, PiplineID, ModelID, LabeledDataID, write, limited),
+  surrogateDataAccess4(Principal, PiplineID, ModelID, full),
+  queryAccess5(Principal, PiplineID, ModelID, decision, limited),
+  trainingDataKnowledge5(Principal, PiplineID, ModelID, TrainingDataID, full),
+  dataPropertiesKnowledge4(Principal, PiplineID, ModelID, full),
+  taskKnowledge4(Principal, PiplineID, ModelID, full).</t>
+  </si>
+  <si>
+    <t>evasionAttack4(Principal, PiplineID, ModelID, tampering) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  modelRetrainedContinuously_p2(PiplineID, ModelID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, evasionAttackVulnerability),
+  rawDataAccess6(Principal, PiplineID, ModelID, RawDataID, write, limited),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, write, limited),
+  labeledDataAccess6(Principal, PiplineID, ModelID, LabeledDataID, write, limited),
+  queryAccess5(Principal, PiplineID, ModelID, decision, limited),
+  completeKnowledge3(Principal, PiplineID, ModelID).</t>
+  </si>
+  <si>
+    <t>evasionAttack4(Principal, PiplineID, ModelID, tampering) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  modelRetrainedContinuously_p2(PiplineID, ModelID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, evasionAttackVulnerability),
+  rawDataAccess6(Principal, PiplineID, ModelID, RawDataID, write, limited),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, write, limited),
+  labeledDataAccess6(Principal, PiplineID,ModelID, LabeledDataID, write, limited),
+  surrogateDataAccess4(Principal, PiplineID, ModelID, full),
+  queryAccess5(Principal, PiplineID, ModelID, decision, limited),
+  trainingDataKnowledge5(Principal, PiplineID, ModelID, TrainingDataID, full),
+  dataPropertiesKnowledge4(Principal, PiplineID, ModelID, full),
+  taskKnowledge4(Principal, PiplineID, ModelID, full).</t>
+  </si>
+  <si>
+    <t>mlModelCorruptionAttack3(Principal, PiplineID, ModelID, tampering_dos) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  modelRetrainedContinuously_p2(PiplineID, ModelID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, evasionAttackVulnerability),
+  rawDataAccess6(Principal, PiplineID, ModelID, RawDataID, write, limited),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, write, limited),
+  labeledDataAccess6(Principal, PiplineID, ModelID, LabeledDataID, write, limited),
+  queryAccess5(Principal, PiplineID, ModelID, decision, limited),
+  completeKnowledge3(Principal, PiplineID, ModelID).</t>
+  </si>
+  <si>
+    <t>mlModelCorruptionAttack3(Principal, PiplineID, ModelID, tampering_dos) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  modelRetrainedContinuously_p2(PiplineID, ModelID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, _),
+  rawDataAccess6(Principal, PiplineID, ModelID, RawDataID, write, limited),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, write, limited),
+  labeledDataAccess6(Principal, PiplineID, ModelID, LabeledDataID, write, limited),
+  surrogateDataAccess4(Principal, PiplineID, ModelID, full),
+  queryAccess5(Principal, PiplineID, ModelID, decision, limited),
+  trainingDataKnowledge5(Principal, PiplineID, ModelID, TrainingDataID, full),
+  dataPropertiesKnowledge4(Principal, PiplineID, ModelID, full),
+  taskKnowledge4(Principal, PiplineID, ModelID, full).</t>
+  </si>
+  <si>
+    <t>membershipInferenceAttack4(Principal, PiplineID, ModelID, informationDisclosure) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, membershipInferenceAttackVulnerability),
+  rawDataAccess6(Principal, PiplineID, ModelID, RawDataID, _, limited),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, _, limited),
+  queryAccess5(Principal, PiplineID, ModelID, decision, full),
+  trainingDataKnowledge5(Principal, PiplineID, ModelID, TrainingDataID, partial),
+  taskKnowledge4(Principal, PiplineID, ModelID, full).</t>
+  </si>
+  <si>
+    <t>membershipInferenceAttack4(Principal, PiplineID, ModelID, informationDisclosure) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  modelRetrainedContinuously_p2(PiplineID, ModelID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, membershipInferenceAttackVulnerability),
+  modelAccess5(Principal, PiplineID, ModelID, _, full),
+  predictionsAccess6(Principal, PiplineID, ModelID, PredictionsDataID, _, full),
+  rawDataAccess6(Principal, PiplineID, ModelID, RawDataID, write, limited),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, write, limited),
+  queryAccess5(Principal, PiplineID, ModelID, score, full),
+  modelKnowledge4(Principal, PiplineID, ModelID, full),
+  hyperparametersKnowledge4(Principal, PiplineID, ModelID, full),
+  algorithmKnowledge4(Principal, PiplineID, ModelID, full),
+  trainingDataKnowledge5(Principal, PiplineID, ModelID, TrainingDataID, partial),
+  taskKnowledge4(Principal, PiplineID, ModelID, full).</t>
+  </si>
+  <si>
+    <t>membershipInferenceAttack4(Principal, PiplineID, ModelID, informationDisclosure) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, membershipInferenceAttackVulnerability),
+  rawDataAccess6(Principal, PiplineID, ModelID, RawDataID, _, full),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID ,_, full),
+  labeledDataAccess6(Principal, PiplineID, ModelID, LabeledDataID, _, full).</t>
+  </si>
+  <si>
+    <t>dataPropertyInferenceAttack4(Principal, PiplineID, ModelID, informationDisclosure) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, dataPropertyInferenceAttackVulnerability),
+  rawDataAccess6(Principal, PiplineID, ModelID, RawDataID, _, limited),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID ,_, limited),
+  queryAccess5(Principal, PiplineID, ModelID, _, full),
+  trainingDataKnowledge5(Principal, PiplineID, ModelID, TrainingDataID, partial),
+  taskKnowledge4(Principal, PiplineID, ModelID, partial).</t>
+  </si>
+  <si>
+    <t>dataPropertyInferenceAttack4(Principal, PiplineID, ModelID, informationDisclosure) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, dataPropertyInferenceAttackVulnerability),
+  rawDataAccess6(Principal, PiplineID, ModelID, RawDataID, _, full),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, _, full),
+  labeledDataAccess6(Principal, PiplineID, ModelID, LabeledDataID, _, full).</t>
+  </si>
+  <si>
+    <t>dataReconstructionAttack4(Principal, PiplineID, ModelID, informationDisclosure) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, dataReconstructionAttackVulnerability),
+  modelAccess5(Principal, PiplineID, ModelID, _, limited),
+  predictionsAccess6(Principal, PiplineID, ModelID, PredictionsDataID, _, limited),
+  rawDataAccess6(Principal, PiplineID, ModelID, RawDataID, _, limited),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, _, limited),
+  queryAccess5(Principal, PiplineID, ModelID, _, full),
+  modelKnowledge4(Principal, PiplineID, ModelID, full),
+  trainingDataKnowledge5(Principal, PiplineID, ModelID, TrainingDataID, partial),
+  rawDataKnowledge5(Principal, PiplineID, ModelID, RawDataID, partial),
+  taskKnowledge4(Principal, PiplineID, ModelID, partial).</t>
+  </si>
+  <si>
+    <t>dataReconstructionAttack4(Principal, PiplineID, ModelID, informationDisclosure) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, dataReconstructionAttackVulnerability),
+  rawDataAccess6(Principal, PiplineID,ModelID, RawDataID, _, limited),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, _, limited),
+  queryAccess5(Principal, PiplineID, ModelID, _, full),
+  trainingDataKnowledge5(Principal, PiplineID, ModelID, TrainingDataID, partial),
+  rawDataKnowledge5(Principal, PiplineID, ModelID, RawDataID, partial),
+  taskKnowledge4(Principal, PiplineID, ModelID, partial).</t>
+  </si>
+  <si>
+    <t>dataReconstructionAttack4(Principal, PiplineID, ModelID, informationDisclosure) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  rawDataAccess6(Principal, PiplineID, ModelID, RawDataID, _, full),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, _, full),
+  labeledDataAccess6(Principal, PiplineID, ModelID, LabeledDataID, _, full).</t>
+  </si>
+  <si>
+    <t>modelExtractionAttack4(Principal, PiplineID, ModelID, informationDisclosure) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, modelExtractionAttackVulnerability),
+  queryAccess5(Principal, PiplineID,ModelID, _, full),
+  trainingDataKnowledge5(Principal, PiplineID, ModelID, TrainingDataID, partial),
+  rawDataKnowledge5(Principal, PiplineID, ModelID, RawDataID, partial),
+  taskKnowledge4(Principal, PiplineID, ModelID, partial).</t>
+  </si>
+  <si>
+    <t>modelExtractionAttack4(Principal, PiplineID, ModelID, informationDisclosure) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, modelExtractionAttackVulnerability),
+  modelAccess5(Principal, PiplineID, ModelID, _, full).</t>
+  </si>
+  <si>
+    <t>labelManipulationAttack3(Principal, PiplineID, ModelID) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, labelManipulationAttackVulnerability),
+  modelRetrainedContinuously_p2(PiplineID, ModelID),
+  completeKnowledge3(Principal, PiplineID, ModelID),
+  manipulateTrainingData3(Principal, PiplineID, ModelID).</t>
+  </si>
+  <si>
+    <t>labelManipulationAttack3(Principal, PiplineID, ModelID) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, labelManipulationAttackVulnerability),
+  modelRetrainedContinuously_p2(PiplineID, ModelID),
+  externalSourceLabeling_p3(TrainingDataID, LabelingServiceId, false),
+  hasAccessToLabelingService_p2(Principal, LabelingServiceId),
+  completeKnowledge3(Principal, PiplineID, ModelID).</t>
+  </si>
+  <si>
+    <t>labelManipulationAttack3(Principal, PiplineID, ModelID) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  vulModel_p5(PiplineID, AlgorithmID, ModelID, ModelHost, labelManipulationAttackVulnerability),
+  modelRetrainedContinuously_p2(PiplineID, ModelID),
+  externalSourceLabeling_p3(TrainingDataID, LabelingServiceId, true),
+  hasAccessToLabelingService_p2(Principal, LabelingServiceId),
+  knowDataValidationMethod_p2(Principal, LabelingServiceId),
+  completeKnowledge3(Principal, PiplineID, ModelID).</t>
+  </si>
+  <si>
+    <t>manipulateTrainingData3(Principal, PiplineID, ModelID) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  trainingData_p2(DataID, TrainingDataHost),
+  accessFile4(Principal, TrainingDataHost, write, TrainingDataID).</t>
+  </si>
+  <si>
+    <t>manipulateTrainingData3(Principal, PiplineID, ModelID) :-
+  malicious_p1(Principal),
+  trainingData_p2(TrainingDataID, TrainingDataHost),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  accessFile4(Principal, InputDataHost, write, InputDataID),
+  dataTransformationJob6(JobID, JobHost, InputDataID, InputDataHost, TrainingDataID, TrainingDataHost).</t>
+  </si>
+  <si>
+    <t>manipulateTrainingData3(Principal, PiplineID, ModelID) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  accessFile4(Principal, InputDataHost, write, InputDataID),
+  dataTransformationJob6(JobID1, JobHost1, InputDataID, InputDataHost, TransformedDataID, TransformedDataHost),
+  dataTransformationJob6(JobID2, JobHost2, TransformedDataID, TransformedDataHost, TrainingDataID, TrainDataHost).</t>
+  </si>
+  <si>
+    <t>dataTransformationJob6(JobID, WorkerHost, InputDataID, WorkerHost, TransformedDataID, TransformedDataHost) :-
+  dataTransformationJob6(JobID, ClusterGatewayHost, InputDataID, ClusterGatewayHost, TransformedDataID, TransformedDataHost),
+  clusterWorker_p3(WorkerHost, ClusterGatewayHost, ClusterMasterHost).</t>
+  </si>
+  <si>
+    <t>modelAccess5(Principal, PiplineID, ModelID, read, AccessLevel) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  accessFile4(Principal, ModelHost, read, ModelID).</t>
+  </si>
+  <si>
+    <t>modelAccess5(Principal, PiplineID, ModelID, write, AccessLevel) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  accessFile4(Principal, ModelHost, write, ModelID).</t>
+  </si>
+  <si>
+    <t>trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, read, AccessLevel) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  accessFile4(Principal, TrainDataHost, read, TrainingDataID).</t>
+  </si>
+  <si>
+    <t>trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, write, AccessLevel) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  accessFile4(Principal, TrainDataHost, write, TrainingDataID).</t>
+  </si>
+  <si>
+    <t>trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, append, AccessLevel) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  accessFile4(Principal, TrainDataHost, append, TrainingDataID).</t>
+  </si>
+  <si>
+    <t>trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, write, AccessLevel) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  manipulateTrainingData3(Principal, PiplineID, ModelID).</t>
+  </si>
+  <si>
+    <t>queryAccess5(Principal, PiplineID, ModelID, PredictionsGranularity, AccessLevel) :-
+  malicious_p1(Principal),
+  predictionService_p8(PiplineID, ModelID, ServingApiID, PredictionServiceHost, Program, Prot, Port, PredictionsGranularity),
+  netAccess5(Principal, _, PredictionServiceHost, Prot, Port).</t>
+  </si>
+  <si>
+    <t>queryAccess5(Principal, PiplineID, ModelID, PredictionsGranularity, AccessLevel) :-
+  malicious_p1(Principal),
+  predictionService_p8(PiplineID, ModelID, ServingApiID, PredictionServiceHost, Program, Prot, Port, PredictionsGranularity),
+  predictorClientApplication_p5(ClientApiID, ServingApiID, PredictorClientApplicationHost, Program),
+  netAccess5(Principal, _, PredictorClientApplicationHost, Prot, Port).</t>
+  </si>
+  <si>
+    <t>queryAccess5(Principal, PiplineID, ModelID, decision, AccessLevel) :-
+  queryAccess5(Principal, PiplineID, ModelID, score, AccessLevel).</t>
+  </si>
+  <si>
+    <t>queryAccess5(Principal, PiplineID, ModelID, PredictionsGranularity, limited) :-
+  queryAccess5(Principal, PiplineID, ModelID, PredictionsGranularity, full).</t>
+  </si>
+  <si>
+    <t>completeAccess4(Principal, PiplineID, ModelID, DataAccessPrivilege) :-
+  modelAccess5(Principal, PiplineID, ModelID, DataAccessPrivilege, AccessLevel),
+  predictionsAccess6(Principal, PiplineID, ModelID, PredictionsDataID, DataAccessPrivilege, AccessLevel),
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, DataAccessPrivilege, AccessLevel),
+  validationDataAccess6(Principal, PiplineID, ModelID, ValidationDataID, DataAccessPrivilege, AccessLevel).</t>
+  </si>
+  <si>
+    <t>modelKnowledge4(Principal, PiplineID, ModelID, KnowledgeLevel) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  publicModel_p1(ModelID).</t>
+  </si>
+  <si>
+    <t>modelKnowledge4(Principal, PiplineID, ModelID, KnowledgeLevel) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  modelAccess5(Principal, PiplineID, ModelID, _, _).</t>
+  </si>
+  <si>
+    <t>hyperparametersKnowledge4(Principal, PiplineID, ModelID, KnowledgeLevel) :-
+ malicious_p1(Principal),
+ model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+ publicModel_p1(ModelID).</t>
+  </si>
+  <si>
+    <t>hyperparametersKnowledge4(Principal, PiplineID, ModelID, KnowledgeLevel) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  modelAccess5(Principal, PiplineID, ModelID, _, _).</t>
+  </si>
+  <si>
+    <t>algorithmKnowledge4(Principal, PiplineID, ModelID, KnowledgeLevel) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  publicModel_p1(ModelID).</t>
+  </si>
+  <si>
+    <t>algorithmKnowledge4(Principal, PiplineID, ModelID, KnowledgeLevel) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  modelAccess5(Principal, PiplineID, ModelID, read, _).</t>
+  </si>
+  <si>
+    <t>trainingDataKnowledge5(Principal, PiplineID, ModelID, TrainingDataID, KnowledgeLevel) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  dataIsPublic_p1(TrainingDataID).</t>
+  </si>
+  <si>
+    <t>trainingDataKnowledge5(Principal, PiplineID, ModelID, TrainingDataID, KnowledgeLevel) :-
+  trainingDataAccess6(Principal, PiplineID, ModelID, TrainingDataID, DataAccessPrivilege, AccessLevel).</t>
+  </si>
+  <si>
+    <t>completeKnowledge3(Principal, PiplineID, ModelID) :-
+  malicious_p1(Principal),
+  modelKnowledge4(Principal, PiplineID, ModelID, KnowledgeLevel),
+  hyperparametersKnowledge4(Principal, PiplineID, ModelID, KnowledgeLevel),
+  algorithmKnowledge4(Principal, PiplineID, ModelID, KnowledgeLevel),
+  trainingDataKnowledge5(Principal, PiplineID, ModelID, TrainingDataID, KnowledgeLevel),
+  rawDataKnowledge5(Principal, PiplineID, ModelID, RawDataID, KnowledgeLevel),
+  dataPropertiesKnowledge4(Principal, PiplineID, ModelID, KnowledgeLevel),
+  taskKnowledge4(Principal, PiplineID, ModelID, KnowledgeLevel).</t>
+  </si>
+  <si>
+    <t>completeKnowledge3(Principal, PiplineID, ModelID) :-
+  malicious_p1(Principal),
+  completeAccess4(Principal, PiplineID, ModelID, _).</t>
+  </si>
+  <si>
+    <t>createSurrogateModel3(Principal, PiplineID, ModelID) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  queryAccess5(Principal, PiplineID, ModelID, score, AccessLevel).</t>
+  </si>
+  <si>
+    <t>createSurrogateModel3(Principal, PiplineID, ModelID) :-
+  malicious_p1(Principal),
+  model_p7(PiplineID, AlgorithmID, ModelID, ModelHost, TrainingDataID, LabelsDataID, ValidationDataID),
+  trainingDataKnowledge5(Principal, PiplineID, ModelID, TrainingDataID, KnowledgeLevel).</t>
+  </si>
+  <si>
     <t>Number of Enterprise ATT&amp;CK Techniques and Sub-Techniques</t>
   </si>
   <si>
@@ -1402,6 +1844,9 @@
   </si>
   <si>
     <t># Covered</t>
+  </si>
+  <si>
+    <t>% Covered</t>
   </si>
   <si>
     <t># Double Counted</t>
@@ -1475,7 +1920,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1503,19 +1948,13 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1660,7 +2099,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1683,8 +2122,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1714,7 +2158,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1727,6 +2181,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1737,16 +2194,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1760,16 +2209,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1984,7 +2430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W900"/>
+  <dimension ref="A1:W1093"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1995,11 +2441,11 @@
   <cols>
     <col min="1" max="1" width="36.75" customWidth="1"/>
     <col min="2" max="2" width="79.375" customWidth="1"/>
-    <col min="3" max="3" width="17.875" customWidth="1"/>
+    <col min="3" max="3" width="12.75" customWidth="1"/>
     <col min="4" max="23" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.25" customHeight="1">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2011,11 +2457,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
@@ -2088,11 +2534,11 @@
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="47"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
@@ -2137,11 +2583,11 @@
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:23">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="47"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -2274,17 +2720,17 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="60">
-      <c r="A33" s="12"/>
-      <c r="B33" s="13" t="s">
+      <c r="A33" s="13"/>
+      <c r="B33" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="60">
       <c r="A34" s="7"/>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="16" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="9" t="s">
@@ -2292,11 +2738,11 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="46"/>
-      <c r="C35" s="47"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="48"/>
     </row>
     <row r="36" spans="1:3" ht="105">
       <c r="A36" s="7" t="s">
@@ -2385,7 +2831,7 @@
     </row>
     <row r="45" spans="1:3" ht="60">
       <c r="A45" s="7"/>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="16" t="s">
         <v>58</v>
       </c>
       <c r="C45" s="9" t="s">
@@ -2394,7 +2840,7 @@
     </row>
     <row r="46" spans="1:3" ht="45">
       <c r="A46" s="7"/>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="17" t="s">
         <v>59</v>
       </c>
       <c r="C46" s="9" t="s">
@@ -2403,7 +2849,7 @@
     </row>
     <row r="47" spans="1:3" ht="60">
       <c r="A47" s="7"/>
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="17" t="s">
         <v>61</v>
       </c>
       <c r="C47" s="9" t="s">
@@ -2414,8 +2860,8 @@
       <c r="A48" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="19"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="7" t="s">
@@ -2491,7 +2937,7 @@
     </row>
     <row r="57" spans="1:3" ht="60">
       <c r="A57" s="7"/>
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="16" t="s">
         <v>58</v>
       </c>
       <c r="C57" s="9" t="s">
@@ -2506,11 +2952,11 @@
       <c r="C58" s="9"/>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="45" t="s">
+      <c r="A59" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="B59" s="46"/>
-      <c r="C59" s="47"/>
+      <c r="B59" s="47"/>
+      <c r="C59" s="48"/>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="7" t="s">
@@ -2576,7 +3022,7 @@
       <c r="C68" s="9"/>
     </row>
     <row r="69" spans="1:3" ht="60">
-      <c r="A69" s="19" t="s">
+      <c r="A69" s="20" t="s">
         <v>33</v>
       </c>
       <c r="B69" s="8" t="s">
@@ -2615,7 +3061,7 @@
       <c r="C73" s="9"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="20" t="s">
         <v>64</v>
       </c>
       <c r="B74" s="11"/>
@@ -2636,7 +3082,7 @@
       <c r="C76" s="9"/>
     </row>
     <row r="77" spans="1:3" ht="60">
-      <c r="A77" s="19" t="s">
+      <c r="A77" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B77" s="8" t="s">
@@ -2647,17 +3093,17 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="60">
-      <c r="A78" s="19"/>
-      <c r="B78" s="13" t="s">
+      <c r="A78" s="20"/>
+      <c r="B78" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C78" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="60">
-      <c r="A79" s="19"/>
-      <c r="B79" s="15" t="s">
+      <c r="A79" s="20"/>
+      <c r="B79" s="16" t="s">
         <v>44</v>
       </c>
       <c r="C79" s="9" t="s">
@@ -2665,11 +3111,11 @@
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="45" t="s">
+      <c r="A80" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="B80" s="46"/>
-      <c r="C80" s="47"/>
+      <c r="B80" s="47"/>
+      <c r="C80" s="48"/>
     </row>
     <row r="81" spans="1:3" ht="90">
       <c r="A81" s="7" t="s">
@@ -2690,28 +3136,28 @@
       <c r="C82" s="9"/>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="19" t="s">
+      <c r="A83" s="20" t="s">
         <v>75</v>
       </c>
       <c r="B83" s="11"/>
       <c r="C83" s="9"/>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="19" t="s">
+      <c r="A84" s="20" t="s">
         <v>76</v>
       </c>
       <c r="B84" s="11"/>
       <c r="C84" s="9"/>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="19" t="s">
+      <c r="A85" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B85" s="11"/>
       <c r="C85" s="9"/>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="19" t="s">
+      <c r="A86" s="20" t="s">
         <v>81</v>
       </c>
       <c r="B86" s="11"/>
@@ -2811,7 +3257,7 @@
     </row>
     <row r="97" spans="1:3" ht="60">
       <c r="A97" s="7"/>
-      <c r="B97" s="16" t="s">
+      <c r="B97" s="17" t="s">
         <v>99</v>
       </c>
       <c r="C97" s="9" t="s">
@@ -2820,7 +3266,7 @@
     </row>
     <row r="98" spans="1:3" ht="120">
       <c r="A98" s="7"/>
-      <c r="B98" s="16" t="s">
+      <c r="B98" s="17" t="s">
         <v>101</v>
       </c>
       <c r="C98" s="9" t="s">
@@ -2829,7 +3275,7 @@
     </row>
     <row r="99" spans="1:3" ht="45">
       <c r="A99" s="7"/>
-      <c r="B99" s="20" t="s">
+      <c r="B99" s="21" t="s">
         <v>102</v>
       </c>
       <c r="C99" s="9" t="s">
@@ -2844,7 +3290,7 @@
       <c r="C100" s="9"/>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="20" t="s">
         <v>82</v>
       </c>
       <c r="B101" s="11"/>
@@ -2863,7 +3309,7 @@
     </row>
     <row r="103" spans="1:3" ht="60">
       <c r="A103" s="7"/>
-      <c r="B103" s="8" t="s">
+      <c r="B103" s="22" t="s">
         <v>107</v>
       </c>
       <c r="C103" s="9" t="s">
@@ -2871,14 +3317,14 @@
       </c>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="19" t="s">
+      <c r="A104" s="20" t="s">
         <v>64</v>
       </c>
       <c r="B104" s="11"/>
       <c r="C104" s="9"/>
     </row>
     <row r="105" spans="1:3" ht="90">
-      <c r="A105" s="19" t="s">
+      <c r="A105" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B105" s="8" t="s">
@@ -2889,8 +3335,8 @@
       </c>
     </row>
     <row r="106" spans="1:3" ht="60">
-      <c r="A106" s="19"/>
-      <c r="B106" s="15" t="s">
+      <c r="A106" s="20"/>
+      <c r="B106" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C106" s="9" t="s">
@@ -2898,8 +3344,8 @@
       </c>
     </row>
     <row r="107" spans="1:3" ht="60">
-      <c r="A107" s="19"/>
-      <c r="B107" s="15" t="s">
+      <c r="A107" s="20"/>
+      <c r="B107" s="16" t="s">
         <v>58</v>
       </c>
       <c r="C107" s="9" t="s">
@@ -2907,14 +3353,14 @@
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="45" t="s">
+      <c r="A108" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="B108" s="46"/>
-      <c r="C108" s="47"/>
+      <c r="B108" s="47"/>
+      <c r="C108" s="48"/>
     </row>
     <row r="109" spans="1:3" ht="90">
-      <c r="A109" s="19" t="s">
+      <c r="A109" s="20" t="s">
         <v>89</v>
       </c>
       <c r="B109" s="8" t="s">
@@ -2925,14 +3371,14 @@
       </c>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="19" t="s">
+      <c r="A110" s="20" t="s">
         <v>91</v>
       </c>
       <c r="B110" s="11"/>
       <c r="C110" s="9"/>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="19" t="s">
+      <c r="A111" s="20" t="s">
         <v>74</v>
       </c>
       <c r="B111" s="11"/>
@@ -2974,7 +3420,7 @@
       <c r="C116" s="9"/>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="19" t="s">
+      <c r="A117" s="20" t="s">
         <v>104</v>
       </c>
       <c r="B117" s="11"/>
@@ -2988,7 +3434,7 @@
       <c r="C118" s="9"/>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" s="19" t="s">
+      <c r="A119" s="20" t="s">
         <v>82</v>
       </c>
       <c r="B119" s="11"/>
@@ -3065,14 +3511,14 @@
       <c r="C129" s="9"/>
     </row>
     <row r="130" spans="1:3">
-      <c r="A130" s="19" t="s">
+      <c r="A130" s="20" t="s">
         <v>85</v>
       </c>
       <c r="B130" s="11"/>
       <c r="C130" s="9"/>
     </row>
     <row r="131" spans="1:3" ht="75">
-      <c r="A131" s="19" t="s">
+      <c r="A131" s="20" t="s">
         <v>105</v>
       </c>
       <c r="B131" s="8" t="s">
@@ -3083,8 +3529,8 @@
       </c>
     </row>
     <row r="132" spans="1:3" ht="60">
-      <c r="A132" s="19"/>
-      <c r="B132" s="8" t="s">
+      <c r="A132" s="20"/>
+      <c r="B132" s="22" t="s">
         <v>107</v>
       </c>
       <c r="C132" s="9" t="s">
@@ -3134,7 +3580,7 @@
       <c r="C138" s="9"/>
     </row>
     <row r="139" spans="1:3">
-      <c r="A139" s="19" t="s">
+      <c r="A139" s="20" t="s">
         <v>87</v>
       </c>
       <c r="B139" s="11"/>
@@ -3162,7 +3608,7 @@
       <c r="C142" s="9"/>
     </row>
     <row r="143" spans="1:3" ht="60">
-      <c r="A143" s="19" t="s">
+      <c r="A143" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B143" s="8" t="s">
@@ -3173,7 +3619,7 @@
       </c>
     </row>
     <row r="144" spans="1:3" ht="90">
-      <c r="A144" s="19"/>
+      <c r="A144" s="20"/>
       <c r="B144" s="8" t="s">
         <v>37</v>
       </c>
@@ -3182,17 +3628,17 @@
       </c>
     </row>
     <row r="145" spans="1:3" ht="60">
-      <c r="A145" s="19"/>
-      <c r="B145" s="13" t="s">
+      <c r="A145" s="20"/>
+      <c r="B145" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C145" s="14" t="s">
+      <c r="C145" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="60">
-      <c r="A146" s="19"/>
-      <c r="B146" s="15" t="s">
+      <c r="A146" s="20"/>
+      <c r="B146" s="16" t="s">
         <v>44</v>
       </c>
       <c r="C146" s="9" t="s">
@@ -3200,8 +3646,8 @@
       </c>
     </row>
     <row r="147" spans="1:3" ht="60">
-      <c r="A147" s="19"/>
-      <c r="B147" s="15" t="s">
+      <c r="A147" s="20"/>
+      <c r="B147" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C147" s="9" t="s">
@@ -3209,8 +3655,8 @@
       </c>
     </row>
     <row r="148" spans="1:3" ht="60">
-      <c r="A148" s="19"/>
-      <c r="B148" s="15" t="s">
+      <c r="A148" s="20"/>
+      <c r="B148" s="16" t="s">
         <v>58</v>
       </c>
       <c r="C148" s="9" t="s">
@@ -3239,11 +3685,11 @@
       <c r="C151" s="9"/>
     </row>
     <row r="152" spans="1:3">
-      <c r="A152" s="45" t="s">
+      <c r="A152" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="B152" s="46"/>
-      <c r="C152" s="47"/>
+      <c r="B152" s="47"/>
+      <c r="C152" s="48"/>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="7" t="s">
@@ -3285,7 +3731,7 @@
     </row>
     <row r="157" spans="1:3" ht="105">
       <c r="A157" s="7"/>
-      <c r="B157" s="21" t="s">
+      <c r="B157" s="22" t="s">
         <v>144</v>
       </c>
       <c r="C157" s="9" t="s">
@@ -3462,7 +3908,7 @@
       </c>
     </row>
     <row r="177" spans="1:3">
-      <c r="A177" s="19" t="s">
+      <c r="A177" s="20" t="s">
         <v>119</v>
       </c>
       <c r="B177" s="11"/>
@@ -3714,11 +4160,11 @@
       <c r="C204" s="9"/>
     </row>
     <row r="205" spans="1:3">
-      <c r="A205" s="45" t="s">
+      <c r="A205" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="B205" s="46"/>
-      <c r="C205" s="47"/>
+      <c r="B205" s="47"/>
+      <c r="C205" s="48"/>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="7" t="s">
@@ -3795,7 +4241,7 @@
       <c r="C215" s="9"/>
     </row>
     <row r="216" spans="1:3" ht="90">
-      <c r="A216" s="19" t="s">
+      <c r="A216" s="20" t="s">
         <v>166</v>
       </c>
       <c r="B216" s="8" t="s">
@@ -3806,7 +4252,7 @@
       </c>
     </row>
     <row r="217" spans="1:3" ht="105">
-      <c r="A217" s="19"/>
+      <c r="A217" s="20"/>
       <c r="B217" s="8" t="s">
         <v>168</v>
       </c>
@@ -3815,7 +4261,7 @@
       </c>
     </row>
     <row r="218" spans="1:3" ht="135">
-      <c r="A218" s="19"/>
+      <c r="A218" s="20"/>
       <c r="B218" s="8" t="s">
         <v>169</v>
       </c>
@@ -3824,7 +4270,7 @@
       </c>
     </row>
     <row r="219" spans="1:3" ht="90">
-      <c r="A219" s="19"/>
+      <c r="A219" s="20"/>
       <c r="B219" s="8" t="s">
         <v>170</v>
       </c>
@@ -3833,7 +4279,7 @@
       </c>
     </row>
     <row r="220" spans="1:3" ht="75">
-      <c r="A220" s="19"/>
+      <c r="A220" s="20"/>
       <c r="B220" s="8" t="s">
         <v>171</v>
       </c>
@@ -3842,7 +4288,7 @@
       </c>
     </row>
     <row r="221" spans="1:3" ht="75">
-      <c r="A221" s="19"/>
+      <c r="A221" s="20"/>
       <c r="B221" s="8" t="s">
         <v>172</v>
       </c>
@@ -3851,7 +4297,7 @@
       </c>
     </row>
     <row r="222" spans="1:3" ht="135">
-      <c r="A222" s="19"/>
+      <c r="A222" s="20"/>
       <c r="B222" s="8" t="s">
         <v>173</v>
       </c>
@@ -3860,7 +4306,7 @@
       </c>
     </row>
     <row r="223" spans="1:3" ht="90">
-      <c r="A223" s="19"/>
+      <c r="A223" s="20"/>
       <c r="B223" s="8" t="s">
         <v>174</v>
       </c>
@@ -3869,7 +4315,7 @@
       </c>
     </row>
     <row r="224" spans="1:3" ht="150">
-      <c r="A224" s="19"/>
+      <c r="A224" s="20"/>
       <c r="B224" s="8" t="s">
         <v>157</v>
       </c>
@@ -3878,7 +4324,7 @@
       </c>
     </row>
     <row r="225" spans="1:3" ht="45">
-      <c r="A225" s="19"/>
+      <c r="A225" s="20"/>
       <c r="B225" s="8" t="s">
         <v>140</v>
       </c>
@@ -3887,7 +4333,7 @@
       </c>
     </row>
     <row r="226" spans="1:3" ht="45">
-      <c r="A226" s="19"/>
+      <c r="A226" s="20"/>
       <c r="B226" s="8" t="s">
         <v>141</v>
       </c>
@@ -4027,25 +4473,25 @@
       <c r="C243" s="9"/>
     </row>
     <row r="244" spans="1:3">
-      <c r="A244" s="19" t="s">
+      <c r="A244" s="20" t="s">
         <v>134</v>
       </c>
       <c r="B244" s="11"/>
       <c r="C244" s="9"/>
     </row>
     <row r="245" spans="1:3">
-      <c r="A245" s="45" t="s">
+      <c r="A245" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="B245" s="46"/>
-      <c r="C245" s="47"/>
+      <c r="B245" s="47"/>
+      <c r="C245" s="48"/>
     </row>
     <row r="246" spans="1:3" ht="60">
       <c r="A246" s="7" t="s">
         <v>214</v>
       </c>
       <c r="B246" s="8" t="s">
-        <v>107</v>
+        <v>215</v>
       </c>
       <c r="C246" s="9" t="s">
         <v>95</v>
@@ -4053,21 +4499,21 @@
     </row>
     <row r="247" spans="1:3">
       <c r="A247" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B247" s="11"/>
       <c r="C247" s="9"/>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B248" s="11"/>
       <c r="C248" s="9"/>
     </row>
     <row r="249" spans="1:3" ht="75">
       <c r="A249" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B249" s="8" t="s">
         <v>30</v>
@@ -4078,7 +4524,7 @@
     </row>
     <row r="250" spans="1:3" ht="75">
       <c r="A250" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B250" s="8" t="s">
         <v>30</v>
@@ -4090,7 +4536,7 @@
     <row r="251" spans="1:3" ht="75">
       <c r="A251" s="7"/>
       <c r="B251" s="8" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C251" s="9" t="s">
         <v>158</v>
@@ -4099,21 +4545,21 @@
     <row r="252" spans="1:3" ht="60">
       <c r="A252" s="7"/>
       <c r="B252" s="8" t="s">
-        <v>107</v>
+        <v>215</v>
       </c>
       <c r="C252" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="253" spans="1:3">
-      <c r="A253" s="19" t="s">
+      <c r="A253" s="20" t="s">
         <v>38</v>
       </c>
       <c r="B253" s="11"/>
       <c r="C253" s="9"/>
     </row>
     <row r="254" spans="1:3">
-      <c r="A254" s="19" t="s">
+      <c r="A254" s="20" t="s">
         <v>67</v>
       </c>
       <c r="B254" s="11"/>
@@ -4121,77 +4567,77 @@
     </row>
     <row r="255" spans="1:3">
       <c r="A255" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B255" s="11"/>
       <c r="C255" s="9"/>
     </row>
     <row r="256" spans="1:3">
-      <c r="A256" s="19" t="s">
+      <c r="A256" s="20" t="s">
         <v>133</v>
       </c>
       <c r="B256" s="11"/>
       <c r="C256" s="9"/>
     </row>
     <row r="257" spans="1:3">
-      <c r="A257" s="45" t="s">
-        <v>221</v>
-      </c>
-      <c r="B257" s="46"/>
-      <c r="C257" s="47"/>
+      <c r="A257" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="B257" s="47"/>
+      <c r="C257" s="48"/>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B258" s="11"/>
       <c r="C258" s="9"/>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B259" s="11"/>
       <c r="C259" s="9"/>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B260" s="11"/>
       <c r="C260" s="9"/>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B261" s="11"/>
       <c r="C261" s="9"/>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B262" s="11"/>
       <c r="C262" s="9"/>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B263" s="11"/>
       <c r="C263" s="9"/>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B264" s="11"/>
       <c r="C264" s="9"/>
     </row>
     <row r="265" spans="1:3" ht="45">
       <c r="A265" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B265" s="8" t="s">
         <v>176</v>
@@ -4203,7 +4649,7 @@
     <row r="266" spans="1:3" ht="45">
       <c r="A266" s="7"/>
       <c r="B266" s="8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C266" s="9" t="s">
         <v>29</v>
@@ -4212,7 +4658,7 @@
     <row r="267" spans="1:3" ht="45">
       <c r="A267" s="7"/>
       <c r="B267" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C267" s="9" t="s">
         <v>29</v>
@@ -4221,7 +4667,7 @@
     <row r="268" spans="1:3" ht="60">
       <c r="A268" s="7"/>
       <c r="B268" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C268" s="9" t="s">
         <v>29</v>
@@ -4230,7 +4676,7 @@
     <row r="269" spans="1:3" ht="30">
       <c r="A269" s="7"/>
       <c r="B269" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C269" s="9" t="s">
         <v>29</v>
@@ -4239,7 +4685,7 @@
     <row r="270" spans="1:3" ht="45">
       <c r="A270" s="7"/>
       <c r="B270" s="8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C270" s="9" t="s">
         <v>31</v>
@@ -4248,7 +4694,7 @@
     <row r="271" spans="1:3" ht="45">
       <c r="A271" s="7"/>
       <c r="B271" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C271" s="9" t="s">
         <v>26</v>
@@ -4257,7 +4703,7 @@
     <row r="272" spans="1:3" ht="45">
       <c r="A272" s="7"/>
       <c r="B272" s="8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C272" s="9" t="s">
         <v>26</v>
@@ -4266,18 +4712,18 @@
     <row r="273" spans="1:3" ht="60">
       <c r="A273" s="7"/>
       <c r="B273" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C273" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="274" spans="1:3" ht="45">
       <c r="A274" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B274" s="8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C274" s="9" t="s">
         <v>29</v>
@@ -4286,7 +4732,7 @@
     <row r="275" spans="1:3" ht="60">
       <c r="A275" s="7"/>
       <c r="B275" s="8" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C275" s="9" t="s">
         <v>29</v>
@@ -4295,7 +4741,7 @@
     <row r="276" spans="1:3" ht="90">
       <c r="A276" s="7"/>
       <c r="B276" s="8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C276" s="9" t="s">
         <v>29</v>
@@ -4304,7 +4750,7 @@
     <row r="277" spans="1:3" ht="105">
       <c r="A277" s="7"/>
       <c r="B277" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C277" s="9" t="s">
         <v>29</v>
@@ -4313,7 +4759,7 @@
     <row r="278" spans="1:3" ht="45">
       <c r="A278" s="7"/>
       <c r="B278" s="8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C278" s="9" t="s">
         <v>29</v>
@@ -4322,7 +4768,7 @@
     <row r="279" spans="1:3" ht="90">
       <c r="A279" s="7"/>
       <c r="B279" s="8" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C279" s="9" t="s">
         <v>55</v>
@@ -4330,8 +4776,8 @@
     </row>
     <row r="280" spans="1:3" ht="75">
       <c r="A280" s="7"/>
-      <c r="B280" s="16" t="s">
-        <v>246</v>
+      <c r="B280" s="17" t="s">
+        <v>247</v>
       </c>
       <c r="C280" s="9" t="s">
         <v>100</v>
@@ -4339,27 +4785,27 @@
     </row>
     <row r="281" spans="1:3">
       <c r="A281" s="7" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B281" s="11"/>
       <c r="C281" s="9"/>
     </row>
     <row r="282" spans="1:3">
       <c r="A282" s="7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B282" s="11"/>
       <c r="C282" s="9"/>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B283" s="11"/>
       <c r="C283" s="9"/>
     </row>
     <row r="284" spans="1:3">
-      <c r="A284" s="19" t="s">
+      <c r="A284" s="20" t="s">
         <v>146</v>
       </c>
       <c r="B284" s="11"/>
@@ -4367,13 +4813,13 @@
     </row>
     <row r="285" spans="1:3">
       <c r="A285" s="7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B285" s="11"/>
       <c r="C285" s="9"/>
     </row>
     <row r="286" spans="1:3" ht="45">
-      <c r="A286" s="19" t="s">
+      <c r="A286" s="20" t="s">
         <v>147</v>
       </c>
       <c r="B286" s="8" t="s">
@@ -4384,7 +4830,7 @@
       </c>
     </row>
     <row r="287" spans="1:3" ht="75">
-      <c r="A287" s="19"/>
+      <c r="A287" s="20"/>
       <c r="B287" s="8" t="s">
         <v>149</v>
       </c>
@@ -4393,7 +4839,7 @@
       </c>
     </row>
     <row r="288" spans="1:3" ht="75">
-      <c r="A288" s="19"/>
+      <c r="A288" s="20"/>
       <c r="B288" s="8" t="s">
         <v>150</v>
       </c>
@@ -4402,7 +4848,7 @@
       </c>
     </row>
     <row r="289" spans="1:3" ht="75">
-      <c r="A289" s="19"/>
+      <c r="A289" s="20"/>
       <c r="B289" s="8" t="s">
         <v>151</v>
       </c>
@@ -4411,7 +4857,7 @@
       </c>
     </row>
     <row r="290" spans="1:3" ht="75">
-      <c r="A290" s="19"/>
+      <c r="A290" s="20"/>
       <c r="B290" s="8" t="s">
         <v>152</v>
       </c>
@@ -4420,7 +4866,7 @@
       </c>
     </row>
     <row r="291" spans="1:3" ht="75">
-      <c r="A291" s="19"/>
+      <c r="A291" s="20"/>
       <c r="B291" s="8" t="s">
         <v>153</v>
       </c>
@@ -4429,7 +4875,7 @@
       </c>
     </row>
     <row r="292" spans="1:3" ht="75">
-      <c r="A292" s="19"/>
+      <c r="A292" s="20"/>
       <c r="B292" s="8" t="s">
         <v>154</v>
       </c>
@@ -4438,7 +4884,7 @@
       </c>
     </row>
     <row r="293" spans="1:3" ht="45">
-      <c r="A293" s="19"/>
+      <c r="A293" s="20"/>
       <c r="B293" s="8" t="s">
         <v>155</v>
       </c>
@@ -4447,7 +4893,7 @@
       </c>
     </row>
     <row r="294" spans="1:3" ht="45">
-      <c r="A294" s="19"/>
+      <c r="A294" s="20"/>
       <c r="B294" s="8" t="s">
         <v>156</v>
       </c>
@@ -4456,7 +4902,7 @@
       </c>
     </row>
     <row r="295" spans="1:3" ht="150">
-      <c r="A295" s="19"/>
+      <c r="A295" s="20"/>
       <c r="B295" s="8" t="s">
         <v>157</v>
       </c>
@@ -4465,7 +4911,7 @@
       </c>
     </row>
     <row r="296" spans="1:3" ht="90">
-      <c r="A296" s="19"/>
+      <c r="A296" s="20"/>
       <c r="B296" s="8" t="s">
         <v>159</v>
       </c>
@@ -4474,7 +4920,7 @@
       </c>
     </row>
     <row r="297" spans="1:3" ht="105">
-      <c r="A297" s="19"/>
+      <c r="A297" s="20"/>
       <c r="B297" s="8" t="s">
         <v>160</v>
       </c>
@@ -4483,7 +4929,7 @@
       </c>
     </row>
     <row r="298" spans="1:3" ht="105">
-      <c r="A298" s="19"/>
+      <c r="A298" s="20"/>
       <c r="B298" s="8" t="s">
         <v>161</v>
       </c>
@@ -4492,7 +4938,7 @@
       </c>
     </row>
     <row r="299" spans="1:3" ht="75">
-      <c r="A299" s="19"/>
+      <c r="A299" s="20"/>
       <c r="B299" s="8" t="s">
         <v>162</v>
       </c>
@@ -4501,7 +4947,7 @@
       </c>
     </row>
     <row r="300" spans="1:3" ht="60">
-      <c r="A300" s="19"/>
+      <c r="A300" s="20"/>
       <c r="B300" s="8" t="s">
         <v>163</v>
       </c>
@@ -4510,7 +4956,7 @@
       </c>
     </row>
     <row r="301" spans="1:3" ht="60">
-      <c r="A301" s="19"/>
+      <c r="A301" s="20"/>
       <c r="B301" s="8" t="s">
         <v>164</v>
       </c>
@@ -4519,7 +4965,7 @@
       </c>
     </row>
     <row r="302" spans="1:3" ht="60">
-      <c r="A302" s="19"/>
+      <c r="A302" s="20"/>
       <c r="B302" s="8" t="s">
         <v>165</v>
       </c>
@@ -4529,125 +4975,125 @@
     </row>
     <row r="303" spans="1:3">
       <c r="A303" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B303" s="11"/>
       <c r="C303" s="9"/>
     </row>
     <row r="304" spans="1:3">
       <c r="A304" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B304" s="11"/>
       <c r="C304" s="9"/>
     </row>
     <row r="305" spans="1:3">
-      <c r="A305" s="45" t="s">
-        <v>253</v>
-      </c>
-      <c r="B305" s="46"/>
-      <c r="C305" s="47"/>
+      <c r="A305" s="46" t="s">
+        <v>254</v>
+      </c>
+      <c r="B305" s="47"/>
+      <c r="C305" s="48"/>
     </row>
     <row r="306" spans="1:3">
       <c r="A306" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B306" s="11"/>
       <c r="C306" s="9"/>
     </row>
     <row r="307" spans="1:3">
       <c r="A307" s="7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B307" s="11"/>
       <c r="C307" s="9"/>
     </row>
     <row r="308" spans="1:3">
       <c r="A308" s="7" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B308" s="11"/>
       <c r="C308" s="9"/>
     </row>
     <row r="309" spans="1:3">
       <c r="A309" s="7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B309" s="11"/>
       <c r="C309" s="9"/>
     </row>
     <row r="310" spans="1:3">
       <c r="A310" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B310" s="11"/>
       <c r="C310" s="9"/>
     </row>
     <row r="311" spans="1:3">
       <c r="A311" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B311" s="11"/>
       <c r="C311" s="9"/>
     </row>
     <row r="312" spans="1:3">
       <c r="A312" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B312" s="11"/>
       <c r="C312" s="9"/>
     </row>
     <row r="313" spans="1:3">
       <c r="A313" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B313" s="11"/>
       <c r="C313" s="9"/>
     </row>
     <row r="314" spans="1:3">
       <c r="A314" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B314" s="11"/>
       <c r="C314" s="9"/>
     </row>
     <row r="315" spans="1:3">
       <c r="A315" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B315" s="11"/>
       <c r="C315" s="9"/>
     </row>
     <row r="316" spans="1:3">
       <c r="A316" s="7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B316" s="11"/>
       <c r="C316" s="9"/>
     </row>
     <row r="317" spans="1:3">
       <c r="A317" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B317" s="11"/>
       <c r="C317" s="9"/>
     </row>
     <row r="318" spans="1:3">
       <c r="A318" s="7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B318" s="11"/>
       <c r="C318" s="9"/>
     </row>
     <row r="319" spans="1:3">
       <c r="A319" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B319" s="11"/>
       <c r="C319" s="9"/>
     </row>
     <row r="320" spans="1:3">
-      <c r="A320" s="19" t="s">
+      <c r="A320" s="20" t="s">
         <v>87</v>
       </c>
       <c r="B320" s="11"/>
@@ -4655,38 +5101,38 @@
     </row>
     <row r="321" spans="1:3">
       <c r="A321" s="7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B321" s="11"/>
       <c r="C321" s="9"/>
     </row>
     <row r="322" spans="1:3">
-      <c r="A322" s="45" t="s">
-        <v>269</v>
-      </c>
-      <c r="B322" s="46"/>
-      <c r="C322" s="47"/>
+      <c r="A322" s="46" t="s">
+        <v>270</v>
+      </c>
+      <c r="B322" s="47"/>
+      <c r="C322" s="48"/>
     </row>
     <row r="323" spans="1:3">
       <c r="A323" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B323" s="11"/>
       <c r="C323" s="9"/>
     </row>
     <row r="324" spans="1:3">
       <c r="A324" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B324" s="11"/>
       <c r="C324" s="9"/>
     </row>
     <row r="325" spans="1:3" ht="45">
       <c r="A325" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B325" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C325" s="9" t="s">
         <v>57</v>
@@ -4712,17 +5158,17 @@
     </row>
     <row r="328" spans="1:3">
       <c r="A328" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B328" s="11"/>
       <c r="C328" s="9"/>
     </row>
     <row r="329" spans="1:3" ht="60">
       <c r="A329" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="B329" s="16" t="s">
         <v>276</v>
+      </c>
+      <c r="B329" s="17" t="s">
+        <v>277</v>
       </c>
       <c r="C329" s="9" t="s">
         <v>26</v>
@@ -4730,8 +5176,8 @@
     </row>
     <row r="330" spans="1:3" ht="105">
       <c r="A330" s="7"/>
-      <c r="B330" s="16" t="s">
-        <v>277</v>
+      <c r="B330" s="17" t="s">
+        <v>278</v>
       </c>
       <c r="C330" s="9" t="s">
         <v>26</v>
@@ -4739,8 +5185,8 @@
     </row>
     <row r="331" spans="1:3" ht="60">
       <c r="A331" s="7"/>
-      <c r="B331" s="16" t="s">
-        <v>278</v>
+      <c r="B331" s="17" t="s">
+        <v>279</v>
       </c>
       <c r="C331" s="9" t="s">
         <v>26</v>
@@ -4748,8 +5194,8 @@
     </row>
     <row r="332" spans="1:3" ht="75">
       <c r="A332" s="7"/>
-      <c r="B332" s="16" t="s">
-        <v>279</v>
+      <c r="B332" s="17" t="s">
+        <v>280</v>
       </c>
       <c r="C332" s="9" t="s">
         <v>26</v>
@@ -4757,8 +5203,8 @@
     </row>
     <row r="333" spans="1:3" ht="60">
       <c r="A333" s="7"/>
-      <c r="B333" s="16" t="s">
-        <v>280</v>
+      <c r="B333" s="17" t="s">
+        <v>281</v>
       </c>
       <c r="C333" s="9" t="s">
         <v>26</v>
@@ -4766,8 +5212,8 @@
     </row>
     <row r="334" spans="1:3" ht="75">
       <c r="A334" s="7"/>
-      <c r="B334" s="16" t="s">
-        <v>281</v>
+      <c r="B334" s="17" t="s">
+        <v>282</v>
       </c>
       <c r="C334" s="9" t="s">
         <v>26</v>
@@ -4775,7 +5221,7 @@
     </row>
     <row r="335" spans="1:3" ht="75">
       <c r="A335" s="7" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B335" s="8" t="s">
         <v>193</v>
@@ -4786,56 +5232,56 @@
     </row>
     <row r="336" spans="1:3">
       <c r="A336" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B336" s="11"/>
       <c r="C336" s="9"/>
     </row>
     <row r="337" spans="1:3">
-      <c r="A337" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="B337" s="22"/>
-      <c r="C337" s="14"/>
+      <c r="A337" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="B337" s="23"/>
+      <c r="C337" s="15"/>
     </row>
     <row r="338" spans="1:3">
       <c r="A338" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="B338" s="10"/>
+        <v>286</v>
+      </c>
+      <c r="B338" s="24"/>
       <c r="C338" s="9"/>
     </row>
     <row r="339" spans="1:3">
-      <c r="A339" s="45" t="s">
-        <v>286</v>
-      </c>
-      <c r="B339" s="46"/>
-      <c r="C339" s="47"/>
+      <c r="A339" s="46" t="s">
+        <v>287</v>
+      </c>
+      <c r="B339" s="47"/>
+      <c r="C339" s="48"/>
     </row>
     <row r="340" spans="1:3">
       <c r="A340" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B340" s="11"/>
       <c r="C340" s="9"/>
     </row>
     <row r="341" spans="1:3">
       <c r="A341" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B341" s="11"/>
       <c r="C341" s="9"/>
     </row>
     <row r="342" spans="1:3">
       <c r="A342" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B342" s="11"/>
       <c r="C342" s="9"/>
     </row>
     <row r="343" spans="1:3" ht="75">
       <c r="A343" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B343" s="8" t="s">
         <v>106</v>
@@ -4847,7 +5293,7 @@
     <row r="344" spans="1:3" ht="60">
       <c r="A344" s="7"/>
       <c r="B344" s="8" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C344" s="9" t="s">
         <v>57</v>
@@ -4856,7 +5302,7 @@
     <row r="345" spans="1:3" ht="45">
       <c r="A345" s="7"/>
       <c r="B345" s="8" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C345" s="9" t="s">
         <v>57</v>
@@ -4864,17 +5310,17 @@
     </row>
     <row r="346" spans="1:3">
       <c r="A346" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B346" s="11"/>
       <c r="C346" s="9"/>
     </row>
     <row r="347" spans="1:3" ht="45">
       <c r="A347" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B347" s="8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C347" s="9" t="s">
         <v>103</v>
@@ -4882,10 +5328,10 @@
     </row>
     <row r="348" spans="1:3" ht="75">
       <c r="A348" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B348" s="8" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C348" s="9" t="s">
         <v>55</v>
@@ -4894,7 +5340,7 @@
     <row r="349" spans="1:3" ht="45">
       <c r="A349" s="7"/>
       <c r="B349" s="8" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C349" s="9" t="s">
         <v>55</v>
@@ -4903,7 +5349,7 @@
     <row r="350" spans="1:3" ht="60">
       <c r="A350" s="7"/>
       <c r="B350" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C350" s="9" t="s">
         <v>57</v>
@@ -4911,24 +5357,24 @@
     </row>
     <row r="351" spans="1:3">
       <c r="A351" s="7" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B351" s="11"/>
       <c r="C351" s="9"/>
     </row>
     <row r="352" spans="1:3">
       <c r="A352" s="7" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B352" s="11"/>
       <c r="C352" s="9"/>
     </row>
     <row r="353" spans="1:3" ht="90">
       <c r="A353" s="7" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B353" s="8" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C353" s="9" t="s">
         <v>55</v>
@@ -4937,7 +5383,7 @@
     <row r="354" spans="1:3" ht="75">
       <c r="A354" s="7"/>
       <c r="B354" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C354" s="9" t="s">
         <v>57</v>
@@ -4946,7 +5392,7 @@
     <row r="355" spans="1:3" ht="45">
       <c r="A355" s="7"/>
       <c r="B355" s="8" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C355" s="9" t="s">
         <v>26</v>
@@ -4954,8 +5400,8 @@
     </row>
     <row r="356" spans="1:3" ht="60">
       <c r="A356" s="7"/>
-      <c r="B356" s="16" t="s">
-        <v>306</v>
+      <c r="B356" s="17" t="s">
+        <v>307</v>
       </c>
       <c r="C356" s="9" t="s">
         <v>26</v>
@@ -4963,8 +5409,8 @@
     </row>
     <row r="357" spans="1:3" ht="105">
       <c r="A357" s="7"/>
-      <c r="B357" s="16" t="s">
-        <v>307</v>
+      <c r="B357" s="17" t="s">
+        <v>308</v>
       </c>
       <c r="C357" s="9" t="s">
         <v>26</v>
@@ -4972,8 +5418,8 @@
     </row>
     <row r="358" spans="1:3" ht="60">
       <c r="A358" s="7"/>
-      <c r="B358" s="16" t="s">
-        <v>308</v>
+      <c r="B358" s="17" t="s">
+        <v>309</v>
       </c>
       <c r="C358" s="9" t="s">
         <v>26</v>
@@ -4981,8 +5427,8 @@
     </row>
     <row r="359" spans="1:3" ht="75">
       <c r="A359" s="7"/>
-      <c r="B359" s="16" t="s">
-        <v>309</v>
+      <c r="B359" s="17" t="s">
+        <v>310</v>
       </c>
       <c r="C359" s="9" t="s">
         <v>26</v>
@@ -4990,8 +5436,8 @@
     </row>
     <row r="360" spans="1:3" ht="60">
       <c r="A360" s="7"/>
-      <c r="B360" s="16" t="s">
-        <v>310</v>
+      <c r="B360" s="17" t="s">
+        <v>311</v>
       </c>
       <c r="C360" s="9" t="s">
         <v>26</v>
@@ -4999,8 +5445,8 @@
     </row>
     <row r="361" spans="1:3" ht="75">
       <c r="A361" s="7"/>
-      <c r="B361" s="16" t="s">
-        <v>311</v>
+      <c r="B361" s="17" t="s">
+        <v>312</v>
       </c>
       <c r="C361" s="9" t="s">
         <v>26</v>
@@ -5008,36 +5454,36 @@
     </row>
     <row r="362" spans="1:3">
       <c r="A362" s="7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B362" s="11"/>
       <c r="C362" s="9"/>
     </row>
     <row r="363" spans="1:3">
       <c r="A363" s="7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B363" s="11"/>
       <c r="C363" s="9"/>
     </row>
     <row r="364" spans="1:3">
       <c r="A364" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B364" s="11"/>
       <c r="C364" s="9"/>
     </row>
     <row r="365" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A365" s="45" t="s">
-        <v>315</v>
-      </c>
-      <c r="B365" s="46"/>
-      <c r="C365" s="47"/>
+      <c r="A365" s="46" t="s">
+        <v>316</v>
+      </c>
+      <c r="B365" s="47"/>
+      <c r="C365" s="48"/>
     </row>
     <row r="366" spans="1:3" ht="60">
       <c r="A366" s="7"/>
-      <c r="B366" s="16" t="s">
-        <v>316</v>
+      <c r="B366" s="17" t="s">
+        <v>317</v>
       </c>
       <c r="C366" s="9" t="s">
         <v>26</v>
@@ -5045,8 +5491,8 @@
     </row>
     <row r="367" spans="1:3" ht="105">
       <c r="A367" s="7"/>
-      <c r="B367" s="16" t="s">
-        <v>317</v>
+      <c r="B367" s="17" t="s">
+        <v>318</v>
       </c>
       <c r="C367" s="9" t="s">
         <v>26</v>
@@ -5054,8 +5500,8 @@
     </row>
     <row r="368" spans="1:3" ht="60">
       <c r="A368" s="7"/>
-      <c r="B368" s="16" t="s">
-        <v>318</v>
+      <c r="B368" s="17" t="s">
+        <v>319</v>
       </c>
       <c r="C368" s="9" t="s">
         <v>26</v>
@@ -5063,8 +5509,8 @@
     </row>
     <row r="369" spans="1:3" ht="75">
       <c r="A369" s="7"/>
-      <c r="B369" s="16" t="s">
-        <v>319</v>
+      <c r="B369" s="17" t="s">
+        <v>320</v>
       </c>
       <c r="C369" s="9" t="s">
         <v>26</v>
@@ -5072,8 +5518,8 @@
     </row>
     <row r="370" spans="1:3" ht="60">
       <c r="A370" s="7"/>
-      <c r="B370" s="16" t="s">
-        <v>320</v>
+      <c r="B370" s="17" t="s">
+        <v>321</v>
       </c>
       <c r="C370" s="9" t="s">
         <v>26</v>
@@ -5081,78 +5527,512 @@
     </row>
     <row r="371" spans="1:3" ht="75">
       <c r="A371" s="7"/>
-      <c r="B371" s="16" t="s">
-        <v>321</v>
+      <c r="B371" s="17" t="s">
+        <v>322</v>
       </c>
       <c r="C371" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="372" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A372" s="7"/>
-      <c r="B372" s="11"/>
-      <c r="C372" s="9"/>
-    </row>
-    <row r="373" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="374" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="375" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="376" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="377" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="378" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="379" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="380" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="381" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="382" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="383" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="384" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
+      <c r="A372" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="B372" s="47"/>
+      <c r="C372" s="48"/>
+    </row>
+    <row r="373" spans="1:3" ht="90">
+      <c r="A373" s="7"/>
+      <c r="B373" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="C373" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" ht="105">
+      <c r="A374" s="7"/>
+      <c r="B374" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="C374" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" ht="105">
+      <c r="A375" s="7"/>
+      <c r="B375" s="25" t="s">
+        <v>327</v>
+      </c>
+      <c r="C375" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" ht="135">
+      <c r="A376" s="7"/>
+      <c r="B376" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="C376" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" ht="150">
+      <c r="A377" s="7"/>
+      <c r="B377" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="C377" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" ht="165">
+      <c r="A378" s="7"/>
+      <c r="B378" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="C378" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" ht="210">
+      <c r="A379" s="7"/>
+      <c r="B379" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="C379" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" ht="165">
+      <c r="A380" s="7"/>
+      <c r="B380" s="25" t="s">
+        <v>332</v>
+      </c>
+      <c r="C380" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" ht="210">
+      <c r="A381" s="7"/>
+      <c r="B381" s="25" t="s">
+        <v>333</v>
+      </c>
+      <c r="C381" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" ht="165">
+      <c r="A382" s="7"/>
+      <c r="B382" s="25" t="s">
+        <v>334</v>
+      </c>
+      <c r="C382" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" ht="210">
+      <c r="A383" s="7"/>
+      <c r="B383" s="25" t="s">
+        <v>335</v>
+      </c>
+      <c r="C383" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" ht="165">
+      <c r="A384" s="7"/>
+      <c r="B384" s="25" t="s">
+        <v>334</v>
+      </c>
+      <c r="C384" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" ht="210">
+      <c r="A385" s="7"/>
+      <c r="B385" s="25" t="s">
+        <v>335</v>
+      </c>
+      <c r="C385" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" ht="165">
+      <c r="A386" s="7"/>
+      <c r="B386" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="C386" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" ht="255">
+      <c r="A387" s="7"/>
+      <c r="B387" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="C387" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" ht="135">
+      <c r="A388" s="7"/>
+      <c r="B388" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="C388" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" ht="165">
+      <c r="A389" s="7"/>
+      <c r="B389" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="C389" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" ht="135">
+      <c r="A390" s="7"/>
+      <c r="B390" s="25" t="s">
+        <v>340</v>
+      </c>
+      <c r="C390" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" ht="225">
+      <c r="A391" s="7"/>
+      <c r="B391" s="25" t="s">
+        <v>341</v>
+      </c>
+      <c r="C391" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" ht="225">
+      <c r="A392" s="7"/>
+      <c r="B392" s="25" t="s">
+        <v>341</v>
+      </c>
+      <c r="C392" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" ht="180">
+      <c r="A393" s="7"/>
+      <c r="B393" s="25" t="s">
+        <v>342</v>
+      </c>
+      <c r="C393" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" ht="105">
+      <c r="A394" s="7"/>
+      <c r="B394" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="C394" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" ht="135">
+      <c r="A395" s="7"/>
+      <c r="B395" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="C395" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" ht="90">
+      <c r="A396" s="7"/>
+      <c r="B396" s="25" t="s">
+        <v>345</v>
+      </c>
+      <c r="C396" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" ht="135">
+      <c r="A397" s="7"/>
+      <c r="B397" s="25" t="s">
+        <v>346</v>
+      </c>
+      <c r="C397" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" ht="150">
+      <c r="A398" s="7"/>
+      <c r="B398" s="25" t="s">
+        <v>347</v>
+      </c>
+      <c r="C398" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" ht="165">
+      <c r="A399" s="7"/>
+      <c r="B399" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="C399" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" ht="90">
+      <c r="A400" s="7"/>
+      <c r="B400" s="25" t="s">
+        <v>349</v>
+      </c>
+      <c r="C400" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" ht="120">
+      <c r="A401" s="7"/>
+      <c r="B401" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="C401" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" ht="135">
+      <c r="A402" s="7"/>
+      <c r="B402" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="C402" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" ht="75">
+      <c r="A403" s="7"/>
+      <c r="B403" s="25" t="s">
+        <v>352</v>
+      </c>
+      <c r="C403" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" ht="75">
+      <c r="A404" s="7"/>
+      <c r="B404" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="C404" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" ht="75">
+      <c r="A405" s="7"/>
+      <c r="B405" s="25" t="s">
+        <v>354</v>
+      </c>
+      <c r="C405" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" ht="75">
+      <c r="A406" s="7"/>
+      <c r="B406" s="25" t="s">
+        <v>355</v>
+      </c>
+      <c r="C406" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" ht="75">
+      <c r="A407" s="7"/>
+      <c r="B407" s="25" t="s">
+        <v>356</v>
+      </c>
+      <c r="C407" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" ht="75">
+      <c r="A408" s="7"/>
+      <c r="B408" s="25" t="s">
+        <v>357</v>
+      </c>
+      <c r="C408" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" ht="75">
+      <c r="A409" s="7"/>
+      <c r="B409" s="25" t="s">
+        <v>358</v>
+      </c>
+      <c r="C409" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" ht="75">
+      <c r="A410" s="7"/>
+      <c r="B410" s="25" t="s">
+        <v>359</v>
+      </c>
+      <c r="C410" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" ht="105">
+      <c r="A411" s="7"/>
+      <c r="B411" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="C411" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" ht="30">
+      <c r="A412" s="7"/>
+      <c r="B412" s="25" t="s">
+        <v>361</v>
+      </c>
+      <c r="C412" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" ht="30">
+      <c r="A413" s="7"/>
+      <c r="B413" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="C413" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" ht="120">
+      <c r="A414" s="7"/>
+      <c r="B414" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="C414" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" ht="75">
+      <c r="A415" s="7"/>
+      <c r="B415" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="C415" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" ht="75">
+      <c r="A416" s="7"/>
+      <c r="B416" s="25" t="s">
+        <v>365</v>
+      </c>
+      <c r="C416" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" ht="75">
+      <c r="A417" s="7"/>
+      <c r="B417" s="25" t="s">
+        <v>366</v>
+      </c>
+      <c r="C417" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" ht="75">
+      <c r="A418" s="7"/>
+      <c r="B418" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="C418" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" ht="75">
+      <c r="A419" s="7"/>
+      <c r="B419" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="C419" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" ht="75">
+      <c r="A420" s="7"/>
+      <c r="B420" s="25" t="s">
+        <v>369</v>
+      </c>
+      <c r="C420" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" ht="75">
+      <c r="A421" s="7"/>
+      <c r="B421" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="C421" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" ht="45">
+      <c r="A422" s="7"/>
+      <c r="B422" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="C422" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" ht="135">
+      <c r="A423" s="7"/>
+      <c r="B423" s="25" t="s">
+        <v>372</v>
+      </c>
+      <c r="C423" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3" ht="45">
+      <c r="A424" s="7"/>
+      <c r="B424" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="C424" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" ht="75">
+      <c r="A425" s="7"/>
+      <c r="B425" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="C425" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" ht="75">
+      <c r="A426" s="7"/>
+      <c r="B426" s="27" t="s">
+        <v>375</v>
+      </c>
+      <c r="C426" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="428" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="429" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="430" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="431" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="432" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="433" ht="14.25" customHeight="1"/>
     <row r="434" ht="14.25" customHeight="1"/>
     <row r="435" ht="14.25" customHeight="1"/>
@@ -5621,23 +6501,217 @@
     <row r="898" ht="14.25" customHeight="1"/>
     <row r="899" ht="14.25" customHeight="1"/>
     <row r="900" ht="14.25" customHeight="1"/>
+    <row r="901" ht="14.25" customHeight="1"/>
+    <row r="902" ht="14.25"/>
+    <row r="903" ht="14.25"/>
+    <row r="904" ht="14.25"/>
+    <row r="905" ht="14.25"/>
+    <row r="906" ht="14.25"/>
+    <row r="907" ht="14.25"/>
+    <row r="908" ht="14.25"/>
+    <row r="909" ht="14.25"/>
+    <row r="910" ht="14.25"/>
+    <row r="911" ht="14.25"/>
+    <row r="912" ht="14.25"/>
+    <row r="913" ht="14.25"/>
+    <row r="914" ht="14.25"/>
+    <row r="915" ht="14.25"/>
+    <row r="916" ht="14.25"/>
+    <row r="917" ht="14.25"/>
+    <row r="918" ht="14.25"/>
+    <row r="919" ht="14.25"/>
+    <row r="920" ht="14.25"/>
+    <row r="921" ht="14.25"/>
+    <row r="922" ht="14.25"/>
+    <row r="923" ht="14.25"/>
+    <row r="924" ht="14.25"/>
+    <row r="925" ht="14.25"/>
+    <row r="926" ht="14.25"/>
+    <row r="927" ht="14.25"/>
+    <row r="928" ht="14.25"/>
+    <row r="929" ht="14.25"/>
+    <row r="930" ht="14.25"/>
+    <row r="931" ht="14.25"/>
+    <row r="932" ht="14.25"/>
+    <row r="933" ht="14.25"/>
+    <row r="934" ht="14.25"/>
+    <row r="935" ht="14.25"/>
+    <row r="936" ht="14.25"/>
+    <row r="937" ht="14.25"/>
+    <row r="938" ht="14.25"/>
+    <row r="939" ht="14.25"/>
+    <row r="940" ht="14.25"/>
+    <row r="941" ht="14.25"/>
+    <row r="942" ht="14.25"/>
+    <row r="943" ht="14.25"/>
+    <row r="944" ht="14.25"/>
+    <row r="945" ht="14.25"/>
+    <row r="946" ht="14.25"/>
+    <row r="947" ht="14.25"/>
+    <row r="948" ht="14.25"/>
+    <row r="949" ht="14.25"/>
+    <row r="950" ht="14.25"/>
+    <row r="951" ht="14.25"/>
+    <row r="952" ht="14.25"/>
+    <row r="953" ht="14.25"/>
+    <row r="954" ht="14.25"/>
+    <row r="955" ht="14.25"/>
+    <row r="956" ht="14.25"/>
+    <row r="957" ht="14.25"/>
+    <row r="958" ht="14.25"/>
+    <row r="959" ht="14.25"/>
+    <row r="960" ht="14.25"/>
+    <row r="961" ht="14.25"/>
+    <row r="962" ht="14.25"/>
+    <row r="963" ht="14.25"/>
+    <row r="964" ht="14.25"/>
+    <row r="965" ht="14.25"/>
+    <row r="966" ht="14.25"/>
+    <row r="967" ht="14.25"/>
+    <row r="968" ht="14.25"/>
+    <row r="969" ht="14.25"/>
+    <row r="970" ht="14.25"/>
+    <row r="971" ht="14.25"/>
+    <row r="972" ht="14.25"/>
+    <row r="973" ht="14.25"/>
+    <row r="974" ht="14.25"/>
+    <row r="975" ht="14.25"/>
+    <row r="976" ht="14.25"/>
+    <row r="977" ht="14.25"/>
+    <row r="978" ht="14.25"/>
+    <row r="979" ht="14.25"/>
+    <row r="980" ht="14.25"/>
+    <row r="981" ht="14.25"/>
+    <row r="982" ht="14.25"/>
+    <row r="983" ht="14.25"/>
+    <row r="984" ht="14.25"/>
+    <row r="985" ht="14.25"/>
+    <row r="986" ht="14.25"/>
+    <row r="987" ht="14.25"/>
+    <row r="988" ht="14.25"/>
+    <row r="989" ht="14.25"/>
+    <row r="990" ht="14.25"/>
+    <row r="991" ht="14.25"/>
+    <row r="992" ht="14.25"/>
+    <row r="993" ht="14.25"/>
+    <row r="994" ht="14.25"/>
+    <row r="995" ht="14.25"/>
+    <row r="996" ht="14.25"/>
+    <row r="997" ht="14.25"/>
+    <row r="998" ht="14.25"/>
+    <row r="999" ht="14.25"/>
+    <row r="1000" ht="14.25"/>
+    <row r="1001" ht="14.25"/>
+    <row r="1002" ht="14.25"/>
+    <row r="1003" ht="14.25"/>
+    <row r="1004" ht="14.25"/>
+    <row r="1005" ht="14.25"/>
+    <row r="1006" ht="14.25"/>
+    <row r="1007" ht="14.25"/>
+    <row r="1008" ht="14.25"/>
+    <row r="1009" ht="14.25"/>
+    <row r="1010" ht="14.25"/>
+    <row r="1011" ht="14.25"/>
+    <row r="1012" ht="14.25"/>
+    <row r="1013" ht="14.25"/>
+    <row r="1014" ht="14.25"/>
+    <row r="1015" ht="14.25"/>
+    <row r="1016" ht="14.25"/>
+    <row r="1017" ht="14.25"/>
+    <row r="1018" ht="14.25"/>
+    <row r="1019" ht="14.25"/>
+    <row r="1020" ht="14.25"/>
+    <row r="1021" ht="14.25"/>
+    <row r="1022" ht="14.25"/>
+    <row r="1023" ht="14.25"/>
+    <row r="1024" ht="14.25"/>
+    <row r="1025" ht="14.25"/>
+    <row r="1026" ht="14.25"/>
+    <row r="1027" ht="14.25"/>
+    <row r="1028" ht="14.25"/>
+    <row r="1029" ht="14.25"/>
+    <row r="1030" ht="14.25"/>
+    <row r="1031" ht="14.25"/>
+    <row r="1032" ht="14.25"/>
+    <row r="1033" ht="14.25"/>
+    <row r="1034" ht="14.25"/>
+    <row r="1035" ht="14.25"/>
+    <row r="1036" ht="14.25"/>
+    <row r="1037" ht="14.25"/>
+    <row r="1038" ht="14.25"/>
+    <row r="1039" ht="14.25"/>
+    <row r="1040" ht="14.25"/>
+    <row r="1041" ht="14.25"/>
+    <row r="1042" ht="14.25"/>
+    <row r="1043" ht="14.25"/>
+    <row r="1044" ht="14.25"/>
+    <row r="1045" ht="14.25"/>
+    <row r="1046" ht="14.25"/>
+    <row r="1047" ht="14.25"/>
+    <row r="1048" ht="14.25"/>
+    <row r="1049" ht="14.25"/>
+    <row r="1050" ht="14.25"/>
+    <row r="1051" ht="14.25"/>
+    <row r="1052" ht="14.25"/>
+    <row r="1053" ht="14.25"/>
+    <row r="1054" ht="14.25"/>
+    <row r="1055" ht="14.25"/>
+    <row r="1056" ht="14.25"/>
+    <row r="1057" ht="14.25"/>
+    <row r="1058" ht="14.25"/>
+    <row r="1059" ht="14.25"/>
+    <row r="1060" ht="14.25"/>
+    <row r="1061" ht="14.25"/>
+    <row r="1062" ht="14.25"/>
+    <row r="1063" ht="14.25"/>
+    <row r="1064" ht="14.25"/>
+    <row r="1065" ht="14.25"/>
+    <row r="1066" ht="14.25"/>
+    <row r="1067" ht="14.25"/>
+    <row r="1068" ht="14.25"/>
+    <row r="1069" ht="14.25"/>
+    <row r="1070" ht="14.25"/>
+    <row r="1071" ht="14.25"/>
+    <row r="1072" ht="14.25"/>
+    <row r="1073" ht="14.25"/>
+    <row r="1074" ht="14.25"/>
+    <row r="1075" ht="14.25"/>
+    <row r="1076" ht="14.25"/>
+    <row r="1077" ht="14.25"/>
+    <row r="1078" ht="14.25"/>
+    <row r="1079" ht="14.25"/>
+    <row r="1080" ht="14.25"/>
+    <row r="1081" ht="14.25"/>
+    <row r="1082" ht="14.25"/>
+    <row r="1083" ht="14.25"/>
+    <row r="1084" ht="14.25"/>
+    <row r="1085" ht="14.25"/>
+    <row r="1086" ht="14.25"/>
+    <row r="1087" ht="14.25"/>
+    <row r="1088" ht="14.25"/>
+    <row r="1089" ht="14.25"/>
+    <row r="1090" ht="14.25"/>
+    <row r="1091" ht="14.25"/>
+    <row r="1092" ht="14.25"/>
+    <row r="1093" ht="14.25"/>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="A108:C108"/>
+    <mergeCell ref="A365:C365"/>
+    <mergeCell ref="A372:C372"/>
+    <mergeCell ref="A152:C152"/>
+    <mergeCell ref="A205:C205"/>
+    <mergeCell ref="A245:C245"/>
+    <mergeCell ref="A257:C257"/>
+    <mergeCell ref="A305:C305"/>
     <mergeCell ref="A322:C322"/>
     <mergeCell ref="A339:C339"/>
-    <mergeCell ref="A365:C365"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="A108:C108"/>
-    <mergeCell ref="A152:C152"/>
-    <mergeCell ref="A205:C205"/>
-    <mergeCell ref="A245:C245"/>
-    <mergeCell ref="A257:C257"/>
-    <mergeCell ref="A305:C305"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -5646,7 +6720,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1002"/>
+  <dimension ref="A1:I1002"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5654,480 +6728,544 @@
   <cols>
     <col min="1" max="1" width="19.625" customWidth="1"/>
     <col min="2" max="2" width="12.875" customWidth="1"/>
-    <col min="3" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="11.875" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="27" width="8.625" customWidth="1"/>
+    <col min="3" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="11.875" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="28" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A1" s="23" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:8" ht="14.25" customHeight="1">
+    <row r="1" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A1" s="28" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:9" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>324</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>325</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>326</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>327</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>325</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>328</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A4" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>379</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>380</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>382</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>379</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>383</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="31">
         <v>10</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="32">
         <v>0</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="33">
+        <f t="shared" ref="D4:D18" si="0">C4/B4</f>
         <v>0</v>
       </c>
-      <c r="E4" s="26">
-        <f t="shared" ref="E4:E17" si="0">B4-D4</f>
+      <c r="E4" s="31">
+        <v>0</v>
+      </c>
+      <c r="F4" s="31">
+        <f t="shared" ref="F4:F17" si="1">B4-E4</f>
         <v>10</v>
       </c>
-      <c r="F4" s="26">
+      <c r="G4" s="31">
         <v>0</v>
       </c>
-      <c r="G4" s="26">
+      <c r="H4" s="31">
         <v>31</v>
       </c>
-      <c r="H4" s="26">
+      <c r="I4" s="31">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="31">
         <v>6</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="32">
         <v>0</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="33">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="31">
+        <v>0</v>
+      </c>
+      <c r="F5" s="31">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G5" s="31">
+        <v>0</v>
+      </c>
+      <c r="H5" s="31">
+        <v>26</v>
+      </c>
+      <c r="I5" s="31">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A6" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="31">
+        <v>9</v>
+      </c>
+      <c r="C6" s="32">
+        <v>5</v>
+      </c>
+      <c r="D6" s="33">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="F5" s="26">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E6" s="31">
         <v>0</v>
       </c>
-      <c r="G5" s="26">
-        <v>26</v>
-      </c>
-      <c r="H5" s="26">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="26">
+      <c r="F6" s="31">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="C6" s="27">
+      <c r="G6" s="31">
         <v>5</v>
       </c>
-      <c r="D6" s="26">
+      <c r="H6" s="31">
+        <v>9</v>
+      </c>
+      <c r="I6" s="31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A7" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="31">
+        <v>10</v>
+      </c>
+      <c r="C7" s="32">
+        <v>5</v>
+      </c>
+      <c r="D7" s="33">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="31">
         <v>0</v>
       </c>
-      <c r="E6" s="26">
+      <c r="F7" s="31">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G7" s="31">
+        <v>5</v>
+      </c>
+      <c r="H7" s="31">
+        <v>18</v>
+      </c>
+      <c r="I7" s="31">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A8" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="31">
+        <v>18</v>
+      </c>
+      <c r="C8" s="32">
+        <v>2</v>
+      </c>
+      <c r="D8" s="33">
         <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="E8" s="31">
+        <v>3</v>
+      </c>
+      <c r="F8" s="31">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="G8" s="31">
+        <v>0</v>
+      </c>
+      <c r="H8" s="31">
+        <v>71</v>
+      </c>
+      <c r="I8" s="31">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A9" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="31">
+        <v>12</v>
+      </c>
+      <c r="C9" s="32">
+        <v>4</v>
+      </c>
+      <c r="D9" s="33">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E9" s="31">
+        <v>7</v>
+      </c>
+      <c r="F9" s="31">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G9" s="31">
+        <v>3</v>
+      </c>
+      <c r="H9" s="31">
+        <v>74</v>
+      </c>
+      <c r="I9" s="31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A10" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="31">
+        <v>37</v>
+      </c>
+      <c r="C10" s="32">
+        <v>3</v>
+      </c>
+      <c r="D10" s="33">
+        <f t="shared" si="0"/>
+        <v>8.1081081081081086E-2</v>
+      </c>
+      <c r="E10" s="31">
         <v>9</v>
       </c>
-      <c r="F6" s="26">
-        <v>5</v>
-      </c>
-      <c r="G6" s="26">
-        <v>9</v>
-      </c>
-      <c r="H6" s="26">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A7" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="26">
-        <v>10</v>
-      </c>
-      <c r="C7" s="27">
-        <v>5</v>
-      </c>
-      <c r="D7" s="26">
-        <v>0</v>
-      </c>
-      <c r="E7" s="26">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F7" s="26">
-        <v>5</v>
-      </c>
-      <c r="G7" s="26">
-        <v>18</v>
-      </c>
-      <c r="H7" s="26">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A8" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="26">
-        <v>18</v>
-      </c>
-      <c r="C8" s="27">
-        <v>2</v>
-      </c>
-      <c r="D8" s="26">
-        <v>3</v>
-      </c>
-      <c r="E8" s="26">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="F8" s="26">
-        <v>0</v>
-      </c>
-      <c r="G8" s="26">
-        <v>71</v>
-      </c>
-      <c r="H8" s="26">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A9" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="26">
-        <v>12</v>
-      </c>
-      <c r="C9" s="27">
-        <v>4</v>
-      </c>
-      <c r="D9" s="26">
-        <v>7</v>
-      </c>
-      <c r="E9" s="26">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F9" s="26">
-        <v>3</v>
-      </c>
-      <c r="G9" s="26">
-        <v>74</v>
-      </c>
-      <c r="H9" s="26">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A10" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="26">
-        <v>37</v>
-      </c>
-      <c r="C10" s="27">
-        <v>3</v>
-      </c>
-      <c r="D10" s="26">
-        <v>9</v>
-      </c>
-      <c r="E10" s="26">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="F10" s="26">
-        <v>0</v>
-      </c>
-      <c r="G10" s="26">
-        <v>102</v>
-      </c>
-      <c r="H10" s="26">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A11" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="B11" s="26">
-        <v>14</v>
-      </c>
-      <c r="C11" s="27">
-        <v>7</v>
-      </c>
-      <c r="D11" s="26">
-        <v>1</v>
-      </c>
-      <c r="E11" s="26">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="F11" s="26">
-        <v>7</v>
-      </c>
-      <c r="G11" s="26">
-        <v>31</v>
-      </c>
-      <c r="H11" s="26">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A12" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B12" s="26">
-        <v>25</v>
-      </c>
-      <c r="C12" s="27">
-        <v>3</v>
-      </c>
-      <c r="D12" s="26">
-        <v>2</v>
-      </c>
-      <c r="E12" s="26">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="F12" s="26">
-        <v>2</v>
-      </c>
-      <c r="G12" s="26">
-        <v>9</v>
-      </c>
-      <c r="H12" s="26">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A13" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="B13" s="26">
-        <v>9</v>
-      </c>
-      <c r="C13" s="27">
-        <v>3</v>
-      </c>
-      <c r="D13" s="26">
-        <v>3</v>
-      </c>
-      <c r="E13" s="26">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="F13" s="26">
-        <v>3</v>
-      </c>
-      <c r="G13" s="26">
-        <v>10</v>
-      </c>
-      <c r="H13" s="26">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A14" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="B14" s="26">
-        <v>17</v>
-      </c>
-      <c r="C14" s="27">
-        <v>3</v>
-      </c>
-      <c r="D14" s="26">
-        <v>2</v>
-      </c>
-      <c r="E14" s="26">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="F14" s="26">
-        <v>2</v>
-      </c>
-      <c r="G14" s="26">
-        <v>13</v>
-      </c>
-      <c r="H14" s="26">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A15" s="28" t="s">
-        <v>253</v>
-      </c>
-      <c r="B15" s="26">
-        <v>16</v>
-      </c>
-      <c r="C15" s="27">
-        <v>0</v>
-      </c>
-      <c r="D15" s="26">
-        <v>1</v>
-      </c>
-      <c r="E15" s="26">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="F15" s="26">
-        <v>0</v>
-      </c>
-      <c r="G15" s="26">
-        <v>22</v>
-      </c>
-      <c r="H15" s="26">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A16" s="28" t="s">
-        <v>269</v>
-      </c>
-      <c r="B16" s="26">
-        <v>9</v>
-      </c>
-      <c r="C16" s="27">
-        <v>3</v>
-      </c>
-      <c r="D16" s="26">
-        <v>0</v>
-      </c>
-      <c r="E16" s="26">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="F16" s="26">
-        <v>3</v>
-      </c>
-      <c r="G16" s="26">
-        <v>7</v>
-      </c>
-      <c r="H16" s="26">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A17" s="28" t="s">
-        <v>286</v>
-      </c>
-      <c r="B17" s="26">
-        <v>13</v>
-      </c>
-      <c r="C17" s="27">
-        <v>4</v>
-      </c>
-      <c r="D17" s="26">
-        <v>0</v>
-      </c>
-      <c r="E17" s="26">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="F17" s="26">
-        <v>4</v>
-      </c>
-      <c r="G17" s="26">
-        <v>13</v>
-      </c>
-      <c r="H17" s="26">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A18" s="29" t="s">
-        <v>330</v>
-      </c>
-      <c r="B18" s="24">
-        <f t="shared" ref="B18:H18" si="1">SUM(B4:B17)</f>
-        <v>205</v>
-      </c>
-      <c r="C18" s="24">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="D18" s="24">
+      <c r="F10" s="31">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="E18" s="24">
+      <c r="G10" s="31">
+        <v>0</v>
+      </c>
+      <c r="H10" s="31">
+        <v>102</v>
+      </c>
+      <c r="I10" s="31">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A11" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="31">
+        <v>14</v>
+      </c>
+      <c r="C11" s="32">
+        <v>7</v>
+      </c>
+      <c r="D11" s="33">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="31">
+        <v>1</v>
+      </c>
+      <c r="F11" s="31">
         <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="G11" s="31">
+        <v>7</v>
+      </c>
+      <c r="H11" s="31">
+        <v>31</v>
+      </c>
+      <c r="I11" s="31">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A12" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="31">
+        <v>25</v>
+      </c>
+      <c r="C12" s="32">
+        <v>3</v>
+      </c>
+      <c r="D12" s="33">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="E12" s="31">
+        <v>2</v>
+      </c>
+      <c r="F12" s="31">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="G12" s="31">
+        <v>2</v>
+      </c>
+      <c r="H12" s="31">
+        <v>9</v>
+      </c>
+      <c r="I12" s="31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A13" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="B13" s="31">
+        <v>9</v>
+      </c>
+      <c r="C13" s="32">
+        <v>3</v>
+      </c>
+      <c r="D13" s="33">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E13" s="31">
+        <v>3</v>
+      </c>
+      <c r="F13" s="31">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G13" s="31">
+        <v>3</v>
+      </c>
+      <c r="H13" s="31">
+        <v>10</v>
+      </c>
+      <c r="I13" s="31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A14" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" s="31">
+        <v>17</v>
+      </c>
+      <c r="C14" s="32">
+        <v>3</v>
+      </c>
+      <c r="D14" s="33">
+        <f t="shared" si="0"/>
+        <v>0.17647058823529413</v>
+      </c>
+      <c r="E14" s="31">
+        <v>2</v>
+      </c>
+      <c r="F14" s="31">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="G14" s="31">
+        <v>2</v>
+      </c>
+      <c r="H14" s="31">
+        <v>13</v>
+      </c>
+      <c r="I14" s="31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A15" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="B15" s="31">
+        <v>16</v>
+      </c>
+      <c r="C15" s="32">
+        <v>0</v>
+      </c>
+      <c r="D15" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="31">
+        <v>1</v>
+      </c>
+      <c r="F15" s="31">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="G15" s="31">
+        <v>0</v>
+      </c>
+      <c r="H15" s="31">
+        <v>22</v>
+      </c>
+      <c r="I15" s="31">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A16" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="B16" s="31">
+        <v>9</v>
+      </c>
+      <c r="C16" s="32">
+        <v>3</v>
+      </c>
+      <c r="D16" s="33">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E16" s="31">
+        <v>0</v>
+      </c>
+      <c r="F16" s="31">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G16" s="31">
+        <v>3</v>
+      </c>
+      <c r="H16" s="31">
+        <v>7</v>
+      </c>
+      <c r="I16" s="31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A17" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="B17" s="31">
+        <v>13</v>
+      </c>
+      <c r="C17" s="32">
+        <v>4</v>
+      </c>
+      <c r="D17" s="33">
+        <f t="shared" si="0"/>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="E17" s="31">
+        <v>0</v>
+      </c>
+      <c r="F17" s="31">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="G17" s="31">
+        <v>4</v>
+      </c>
+      <c r="H17" s="31">
+        <v>13</v>
+      </c>
+      <c r="I17" s="31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A18" s="35" t="s">
+        <v>385</v>
+      </c>
+      <c r="B18" s="29">
+        <f t="shared" ref="B18:C18" si="2">SUM(B4:B17)</f>
+        <v>205</v>
+      </c>
+      <c r="C18" s="29">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="D18" s="33">
+        <f t="shared" si="0"/>
+        <v>0.20487804878048779</v>
+      </c>
+      <c r="E18" s="29">
+        <f t="shared" ref="E18:I18" si="3">SUM(E4:E17)</f>
+        <v>28</v>
+      </c>
+      <c r="F18" s="29">
+        <f t="shared" si="3"/>
         <v>177</v>
       </c>
-      <c r="F18" s="24">
-        <f t="shared" si="1"/>
+      <c r="G18" s="29">
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="G18" s="24">
-        <f t="shared" si="1"/>
+      <c r="H18" s="29">
+        <f t="shared" si="3"/>
         <v>436</v>
       </c>
-      <c r="H18" s="24">
-        <f t="shared" si="1"/>
+      <c r="I18" s="29">
+        <f t="shared" si="3"/>
         <v>322</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.25" customHeight="1">
-      <c r="C19" s="30">
+    <row r="19" spans="1:9" ht="14.25" customHeight="1">
+      <c r="C19" s="36">
         <f>C18/B18</f>
         <v>0.20487804878048779</v>
       </c>
-      <c r="F19" s="30">
-        <f>F18/E18</f>
+      <c r="D19" s="31"/>
+      <c r="G19" s="36">
+        <f>G18/F18</f>
         <v>0.19209039548022599</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:8" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:8" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:8" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:8" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:8" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:8" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:8" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:8" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:8" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:8" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:8" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:8" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:9" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:9" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:9" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:9" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:9" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:9" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:9" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:9" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:9" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:9" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:9" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:9" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:9" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -7110,7 +8248,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -7126,44 +8264,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="31" t="s">
-        <v>331</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>332</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>333</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>334</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>335</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>336</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>337</v>
+      <c r="A1" s="37" t="s">
+        <v>386</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>389</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>390</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>391</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="38" t="s">
         <v>88</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36" t="s">
-        <v>338</v>
-      </c>
-      <c r="G2" s="37"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="G2" s="39"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
@@ -7185,24 +8323,24 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="40" t="s">
-        <v>338</v>
-      </c>
-      <c r="G3" s="41"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="42" t="s">
+        <v>393</v>
+      </c>
+      <c r="G3" s="27"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="38" t="s">
         <v>74</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -7211,30 +8349,30 @@
       <c r="C4" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43" t="s">
-        <v>338</v>
-      </c>
-      <c r="G4" s="41"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="44" t="s">
+        <v>393</v>
+      </c>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="1:26" ht="45">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="40" t="s">
-        <v>339</v>
-      </c>
-      <c r="G5" s="44" t="s">
-        <v>340</v>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="42" t="s">
+        <v>394</v>
+      </c>
+      <c r="G5" s="45" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="45">
@@ -7247,32 +8385,32 @@
       <c r="C6" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="43" t="s">
-        <v>339</v>
-      </c>
-      <c r="G6" s="44" t="s">
-        <v>341</v>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="44" t="s">
+        <v>394</v>
+      </c>
+      <c r="G6" s="45" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="75">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="40" t="s">
-        <v>339</v>
-      </c>
-      <c r="G7" s="44" t="s">
-        <v>342</v>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="42" t="s">
+        <v>394</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="60">
@@ -7285,34 +8423,34 @@
       <c r="C8" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="43" t="s">
-        <v>339</v>
-      </c>
-      <c r="G8" s="44" t="s">
-        <v>343</v>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="44" t="s">
+        <v>394</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="40" t="s">
-        <v>338</v>
-      </c>
-      <c r="G9" s="41"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="42" t="s">
+        <v>393</v>
+      </c>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="38" t="s">
         <v>104</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -7321,31 +8459,31 @@
       <c r="C10" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="43" t="s">
-        <v>338</v>
-      </c>
-      <c r="G10" s="41"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="44" t="s">
+        <v>393</v>
+      </c>
+      <c r="G10" s="27"/>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="40" t="s">
-        <v>338</v>
-      </c>
-      <c r="G11" s="41"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="42" t="s">
+        <v>393</v>
+      </c>
+      <c r="G11" s="27"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="9" t="s">
@@ -7355,31 +8493,31 @@
         <v>137</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="43" t="s">
-        <v>338</v>
-      </c>
-      <c r="G12" s="41"/>
+        <v>222</v>
+      </c>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="44" t="s">
+        <v>393</v>
+      </c>
+      <c r="G12" s="27"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="C13" s="38" t="s">
-        <v>221</v>
-      </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="40" t="s">
-        <v>338</v>
-      </c>
-      <c r="G13" s="41"/>
+      <c r="C13" s="40" t="s">
+        <v>222</v>
+      </c>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="42" t="s">
+        <v>393</v>
+      </c>
+      <c r="G13" s="27"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="9" t="s">
@@ -7391,30 +8529,30 @@
       <c r="C14" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="43" t="s">
-        <v>338</v>
-      </c>
-      <c r="G14" s="41"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="44" t="s">
+        <v>393</v>
+      </c>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="1:26" ht="45">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="40" t="s">
         <v>184</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="40" t="s">
-        <v>339</v>
-      </c>
-      <c r="G15" s="44" t="s">
-        <v>344</v>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="42" t="s">
+        <v>394</v>
+      </c>
+      <c r="G15" s="45" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -7427,32 +8565,32 @@
       <c r="C16" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43" t="s">
-        <v>338</v>
-      </c>
-      <c r="G16" s="41"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="44" t="s">
+        <v>393</v>
+      </c>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="40" t="s">
-        <v>338</v>
-      </c>
-      <c r="G17" s="41"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="42" t="s">
+        <v>393</v>
+      </c>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:7" ht="135">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="38" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -7461,38 +8599,38 @@
       <c r="C18" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="43" t="s">
-        <v>339</v>
-      </c>
-      <c r="G18" s="44" t="s">
-        <v>345</v>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="44" t="s">
+        <v>394</v>
+      </c>
+      <c r="G18" s="45" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="40" t="s">
-        <v>339</v>
-      </c>
-      <c r="G19" s="44" t="s">
-        <v>346</v>
+      <c r="E19" s="40"/>
+      <c r="F19" s="42" t="s">
+        <v>394</v>
+      </c>
+      <c r="G19" s="45" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="38" t="s">
         <v>67</v>
       </c>
       <c r="B20" s="9" t="s">
@@ -7501,31 +8639,31 @@
       <c r="C20" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43" t="s">
-        <v>338</v>
-      </c>
-      <c r="G20" s="41"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="44" t="s">
+        <v>393</v>
+      </c>
+      <c r="G20" s="27"/>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="D21" s="38" t="s">
-        <v>253</v>
-      </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="40" t="s">
-        <v>338</v>
-      </c>
-      <c r="G21" s="41"/>
+      <c r="D21" s="40" t="s">
+        <v>254</v>
+      </c>
+      <c r="E21" s="40"/>
+      <c r="F21" s="42" t="s">
+        <v>393</v>
+      </c>
+      <c r="G21" s="27"/>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1">
       <c r="A22" s="9" t="s">
@@ -7537,34 +8675,34 @@
       <c r="C22" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43" t="s">
-        <v>338</v>
-      </c>
-      <c r="G22" s="41"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="44" t="s">
+        <v>393</v>
+      </c>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:7" ht="90">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="E23" s="38" t="s">
+      <c r="E23" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="F23" s="40" t="s">
-        <v>339</v>
-      </c>
-      <c r="G23" s="44" t="s">
-        <v>347</v>
+      <c r="F23" s="42" t="s">
+        <v>394</v>
+      </c>
+      <c r="G23" s="45" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.25" customHeight="1">
@@ -7577,12 +8715,12 @@
       <c r="C24" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="43" t="s">
-        <v>338</v>
-      </c>
-      <c r="G24" s="41"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44" t="s">
+        <v>393</v>
+      </c>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:7" ht="14.25" customHeight="1"/>

</xml_diff>